<commit_message>
Update: updated for version 1.2
</commit_message>
<xml_diff>
--- a/uploads/xlsx/Timetable SE Department (Fall-25) Version-1.3.xlsx
+++ b/uploads/xlsx/Timetable SE Department (Fall-25) Version-1.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zPythonStuff\Superior Academic Tool\uploads\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3FDCEB-03AD-4D64-B50F-3BC515F3BA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096B62A7-202A-479C-BC05-2D6B7E9DB2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time Table" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="270">
   <si>
     <t>Department fo Software Engineering {Monday to Friday Timetable Fall-25}</t>
   </si>
@@ -2589,6 +2589,9 @@
 BSDS-7A/BSAI-7A
 Ms. Ammara Ejaz</t>
   </si>
+  <si>
+    <t>04:00 - 05:30</t>
+  </si>
 </sst>
 </file>
 
@@ -2598,7 +2601,7 @@
     <numFmt numFmtId="164" formatCode="dddd\ m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="mmmm&quot;-&quot;dd&quot;-&quot;yyyy"/>
   </numFmts>
-  <fonts count="47">
+  <fonts count="46">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2855,11 +2858,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
   </fonts>
@@ -4399,7 +4397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="358">
+  <cellXfs count="357">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4931,7 +4929,197 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="40" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="116" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="117" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="118" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4940,124 +5128,172 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="9" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5075,9 +5311,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5087,10 +5320,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5114,188 +5347,71 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5307,127 +5423,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="40" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="116" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="117" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="118" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5648,9 +5643,9 @@
   </sheetPr>
   <dimension ref="A1:AB999"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
+      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5675,10 +5670,10 @@
       <c r="D1" s="128"/>
       <c r="E1" s="128"/>
       <c r="F1" s="128"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="237"/>
-      <c r="I1" s="237"/>
-      <c r="J1" s="238"/>
+      <c r="G1" s="316"/>
+      <c r="H1" s="317"/>
+      <c r="I1" s="317"/>
+      <c r="J1" s="318"/>
       <c r="K1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -5699,20 +5694,20 @@
       <c r="AB1" s="3"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A2" s="241" t="s">
+      <c r="A2" s="320" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="242"/>
-      <c r="C2" s="242"/>
-      <c r="D2" s="242"/>
-      <c r="E2" s="242"/>
+      <c r="B2" s="321"/>
+      <c r="C2" s="321"/>
+      <c r="D2" s="321"/>
+      <c r="E2" s="321"/>
       <c r="F2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="239"/>
-      <c r="H2" s="239"/>
-      <c r="I2" s="239"/>
-      <c r="J2" s="240"/>
+      <c r="G2" s="310"/>
+      <c r="H2" s="310"/>
+      <c r="I2" s="310"/>
+      <c r="J2" s="319"/>
       <c r="K2" s="1"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -5733,18 +5728,18 @@
       <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A3" s="196"/>
-      <c r="B3" s="243"/>
-      <c r="C3" s="243"/>
-      <c r="D3" s="243"/>
-      <c r="E3" s="244"/>
+      <c r="A3" s="322"/>
+      <c r="B3" s="283"/>
+      <c r="C3" s="283"/>
+      <c r="D3" s="283"/>
+      <c r="E3" s="286"/>
       <c r="F3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="246"/>
-      <c r="H3" s="203"/>
-      <c r="I3" s="203"/>
-      <c r="J3" s="207"/>
+      <c r="G3" s="325"/>
+      <c r="H3" s="301"/>
+      <c r="I3" s="301"/>
+      <c r="J3" s="233"/>
       <c r="K3" s="4"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -5765,18 +5760,18 @@
       <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:28" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A4" s="227"/>
-      <c r="B4" s="245"/>
-      <c r="C4" s="245"/>
-      <c r="D4" s="245"/>
-      <c r="E4" s="245"/>
+      <c r="A4" s="323"/>
+      <c r="B4" s="324"/>
+      <c r="C4" s="324"/>
+      <c r="D4" s="324"/>
+      <c r="E4" s="324"/>
       <c r="F4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="247"/>
-      <c r="H4" s="248"/>
-      <c r="I4" s="248"/>
-      <c r="J4" s="249"/>
+      <c r="G4" s="326"/>
+      <c r="H4" s="327"/>
+      <c r="I4" s="327"/>
+      <c r="J4" s="328"/>
       <c r="K4" s="4"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -5798,10 +5793,10 @@
     </row>
     <row r="5" spans="1:28" ht="27" customHeight="1" thickBot="1">
       <c r="A5" s="129"/>
-      <c r="B5" s="250" t="s">
+      <c r="B5" s="329" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="242"/>
+      <c r="C5" s="321"/>
       <c r="D5" s="146" t="s">
         <v>3</v>
       </c>
@@ -5875,13 +5870,13 @@
       <c r="AB6" s="3"/>
     </row>
     <row r="7" spans="1:28" ht="75" customHeight="1">
-      <c r="A7" s="254" t="s">
+      <c r="A7" s="331" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="258" t="s">
+      <c r="C7" s="263" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="144" t="s">
@@ -5890,17 +5885,17 @@
       <c r="E7" s="144" t="s">
         <v>181</v>
       </c>
-      <c r="F7" s="234" t="s">
+      <c r="F7" s="314" t="s">
         <v>230</v>
       </c>
-      <c r="G7" s="235"/>
+      <c r="G7" s="315"/>
       <c r="H7" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="I7" s="215" t="s">
+      <c r="I7" s="236" t="s">
         <v>215</v>
       </c>
-      <c r="J7" s="207"/>
+      <c r="J7" s="233"/>
       <c r="K7" s="1"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -5921,26 +5916,26 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28" ht="60" customHeight="1">
-      <c r="A8" s="196"/>
+      <c r="A8" s="322"/>
       <c r="B8" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="252"/>
-      <c r="D8" s="266" t="s">
+      <c r="C8" s="264"/>
+      <c r="D8" s="313" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="216"/>
-      <c r="F8" s="232" t="s">
+      <c r="E8" s="239"/>
+      <c r="F8" s="249" t="s">
         <v>220</v>
       </c>
-      <c r="G8" s="233"/>
+      <c r="G8" s="336"/>
       <c r="H8" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="206" t="s">
+      <c r="I8" s="342" t="s">
         <v>193</v>
       </c>
-      <c r="J8" s="207"/>
+      <c r="J8" s="233"/>
       <c r="K8" s="5"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -5961,11 +5956,11 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" ht="61.5" customHeight="1" thickBot="1">
-      <c r="A9" s="196"/>
+      <c r="A9" s="322"/>
       <c r="B9" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="252"/>
+      <c r="C9" s="264"/>
       <c r="D9" s="31" t="s">
         <v>71</v>
       </c>
@@ -5998,11 +5993,11 @@
       <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:28" ht="67.5" customHeight="1">
-      <c r="A10" s="196"/>
+      <c r="A10" s="322"/>
       <c r="B10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="251" t="s">
+      <c r="C10" s="330" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="31" t="s">
@@ -6011,14 +6006,14 @@
       <c r="E10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="219" t="s">
+      <c r="F10" s="227" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="210"/>
-      <c r="H10" s="215" t="s">
+      <c r="G10" s="240"/>
+      <c r="H10" s="236" t="s">
         <v>90</v>
       </c>
-      <c r="I10" s="216"/>
+      <c r="I10" s="239"/>
       <c r="J10" s="102"/>
       <c r="K10" s="3"/>
       <c r="L10" s="2"/>
@@ -6040,25 +6035,25 @@
       <c r="AB10" s="3"/>
     </row>
     <row r="11" spans="1:28" ht="47.25">
-      <c r="A11" s="196"/>
+      <c r="A11" s="322"/>
       <c r="B11" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="252"/>
-      <c r="D11" s="264" t="s">
+      <c r="C11" s="264"/>
+      <c r="D11" s="312" t="s">
         <v>122</v>
       </c>
-      <c r="E11" s="257"/>
+      <c r="E11" s="237"/>
       <c r="F11" s="23" t="s">
         <v>64</v>
       </c>
       <c r="G11" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="219" t="s">
+      <c r="H11" s="227" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="216"/>
+      <c r="I11" s="239"/>
       <c r="J11" s="103"/>
       <c r="K11" s="5"/>
       <c r="L11" s="2"/>
@@ -6080,22 +6075,22 @@
       <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28" ht="87" customHeight="1">
-      <c r="A12" s="196"/>
+      <c r="A12" s="322"/>
       <c r="B12" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="252"/>
-      <c r="D12" s="229" t="s">
+      <c r="C12" s="264"/>
+      <c r="D12" s="279" t="s">
         <v>231</v>
       </c>
-      <c r="E12" s="216"/>
+      <c r="E12" s="239"/>
       <c r="F12" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="219" t="s">
+      <c r="G12" s="227" t="s">
         <v>262</v>
       </c>
-      <c r="H12" s="216"/>
+      <c r="H12" s="239"/>
       <c r="I12" s="23" t="s">
         <v>68</v>
       </c>
@@ -6120,18 +6115,18 @@
       <c r="AB12" s="3"/>
     </row>
     <row r="13" spans="1:28" ht="47.25">
-      <c r="A13" s="196"/>
+      <c r="A13" s="322"/>
       <c r="B13" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="252"/>
+      <c r="C13" s="264"/>
       <c r="D13" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="231" t="s">
+      <c r="E13" s="335" t="s">
         <v>247</v>
       </c>
-      <c r="F13" s="216"/>
+      <c r="F13" s="239"/>
       <c r="G13" s="23" t="s">
         <v>69</v>
       </c>
@@ -6164,11 +6159,11 @@
       <c r="AB13" s="3"/>
     </row>
     <row r="14" spans="1:28" ht="26.25" hidden="1" customHeight="1">
-      <c r="A14" s="196"/>
+      <c r="A14" s="322"/>
       <c r="B14" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="252"/>
+      <c r="C14" s="264"/>
       <c r="D14" s="48"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
@@ -6196,15 +6191,15 @@
       <c r="AB14" s="3"/>
     </row>
     <row r="15" spans="1:28" ht="63">
-      <c r="A15" s="196"/>
+      <c r="A15" s="322"/>
       <c r="B15" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="252"/>
-      <c r="D15" s="264" t="s">
+      <c r="C15" s="264"/>
+      <c r="D15" s="312" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="257"/>
+      <c r="E15" s="237"/>
       <c r="F15" s="51" t="s">
         <v>147</v>
       </c>
@@ -6214,10 +6209,10 @@
       <c r="H15" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="I15" s="215" t="s">
+      <c r="I15" s="236" t="s">
         <v>141</v>
       </c>
-      <c r="J15" s="207"/>
+      <c r="J15" s="233"/>
       <c r="K15" s="5"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -6238,17 +6233,17 @@
       <c r="AB15" s="3"/>
     </row>
     <row r="16" spans="1:28" ht="57.75" customHeight="1">
-      <c r="A16" s="196"/>
+      <c r="A16" s="322"/>
       <c r="B16" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="252"/>
+      <c r="C16" s="264"/>
       <c r="D16" s="49"/>
       <c r="E16" s="37"/>
-      <c r="F16" s="265" t="s">
+      <c r="F16" s="238" t="s">
         <v>196</v>
       </c>
-      <c r="G16" s="225"/>
+      <c r="G16" s="267"/>
       <c r="H16" s="123"/>
       <c r="I16" s="124"/>
       <c r="J16" s="60"/>
@@ -6272,15 +6267,15 @@
       <c r="AB16" s="3"/>
     </row>
     <row r="17" spans="1:28" ht="71.25" customHeight="1">
-      <c r="A17" s="196"/>
+      <c r="A17" s="322"/>
       <c r="B17" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="252"/>
-      <c r="D17" s="202"/>
-      <c r="E17" s="203"/>
-      <c r="F17" s="204"/>
-      <c r="G17" s="205"/>
+      <c r="C17" s="264"/>
+      <c r="D17" s="280"/>
+      <c r="E17" s="301"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="242"/>
       <c r="H17" s="125"/>
       <c r="I17" s="125"/>
       <c r="J17" s="90"/>
@@ -6304,15 +6299,15 @@
       <c r="AB17" s="3"/>
     </row>
     <row r="18" spans="1:28" ht="64.5" customHeight="1">
-      <c r="A18" s="196"/>
+      <c r="A18" s="322"/>
       <c r="B18" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="252"/>
+      <c r="C18" s="264"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="204"/>
-      <c r="G18" s="205"/>
+      <c r="F18" s="253"/>
+      <c r="G18" s="242"/>
       <c r="H18" s="125"/>
       <c r="I18" s="125"/>
       <c r="J18" s="122"/>
@@ -6336,23 +6331,23 @@
       <c r="AB18" s="3"/>
     </row>
     <row r="19" spans="1:28" ht="60.75" customHeight="1">
-      <c r="A19" s="196"/>
+      <c r="A19" s="322"/>
       <c r="B19" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="252"/>
-      <c r="D19" s="229" t="s">
+      <c r="C19" s="264"/>
+      <c r="D19" s="279" t="s">
         <v>113</v>
       </c>
-      <c r="E19" s="216"/>
-      <c r="F19" s="260" t="s">
+      <c r="E19" s="239"/>
+      <c r="F19" s="309" t="s">
         <v>229</v>
       </c>
-      <c r="G19" s="239"/>
-      <c r="H19" s="259" t="s">
+      <c r="G19" s="310"/>
+      <c r="H19" s="241" t="s">
         <v>137</v>
       </c>
-      <c r="I19" s="205"/>
+      <c r="I19" s="242"/>
       <c r="J19" s="90"/>
       <c r="K19" s="5"/>
       <c r="L19" s="2"/>
@@ -6374,23 +6369,23 @@
       <c r="AB19" s="3"/>
     </row>
     <row r="20" spans="1:28" ht="59.25" customHeight="1" thickBot="1">
-      <c r="A20" s="255"/>
+      <c r="A20" s="332"/>
       <c r="B20" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="253"/>
-      <c r="D20" s="261" t="s">
+      <c r="C20" s="265"/>
+      <c r="D20" s="311" t="s">
         <v>159</v>
       </c>
-      <c r="E20" s="201"/>
-      <c r="F20" s="200" t="s">
+      <c r="E20" s="284"/>
+      <c r="F20" s="277" t="s">
         <v>160</v>
       </c>
-      <c r="G20" s="201"/>
-      <c r="H20" s="262" t="s">
+      <c r="G20" s="284"/>
+      <c r="H20" s="293" t="s">
         <v>161</v>
       </c>
-      <c r="I20" s="263"/>
+      <c r="I20" s="294"/>
       <c r="J20" s="85" t="s">
         <v>191</v>
       </c>
@@ -6415,10 +6410,10 @@
     </row>
     <row r="21" spans="1:28" ht="20.25" thickBot="1">
       <c r="A21" s="41"/>
-      <c r="B21" s="223" t="s">
+      <c r="B21" s="351" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="224"/>
+      <c r="C21" s="262"/>
       <c r="D21" s="27"/>
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
@@ -6446,7 +6441,7 @@
       <c r="AB21" s="3"/>
     </row>
     <row r="22" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A22" s="191" t="s">
+      <c r="A22" s="337" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="91" t="s">
@@ -6494,25 +6489,25 @@
       <c r="AB22" s="3"/>
     </row>
     <row r="23" spans="1:28" ht="47.25" customHeight="1">
-      <c r="A23" s="192"/>
+      <c r="A23" s="256"/>
       <c r="B23" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="226" t="s">
+      <c r="C23" s="352" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="211" t="s">
+      <c r="D23" s="344" t="s">
         <v>212</v>
       </c>
-      <c r="E23" s="212"/>
-      <c r="F23" s="213" t="s">
+      <c r="E23" s="345"/>
+      <c r="F23" s="346" t="s">
         <v>138</v>
       </c>
-      <c r="G23" s="212"/>
-      <c r="H23" s="214" t="s">
+      <c r="G23" s="345"/>
+      <c r="H23" s="347" t="s">
         <v>177</v>
       </c>
-      <c r="I23" s="212"/>
+      <c r="I23" s="345"/>
       <c r="J23" s="99" t="s">
         <v>12</v>
       </c>
@@ -6536,23 +6531,23 @@
       <c r="AB23" s="3"/>
     </row>
     <row r="24" spans="1:28" ht="52.5" customHeight="1">
-      <c r="A24" s="192"/>
+      <c r="A24" s="256"/>
       <c r="B24" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="196"/>
-      <c r="D24" s="215" t="s">
+      <c r="C24" s="322"/>
+      <c r="D24" s="236" t="s">
         <v>208</v>
       </c>
-      <c r="E24" s="216"/>
-      <c r="F24" s="215" t="s">
+      <c r="E24" s="239"/>
+      <c r="F24" s="236" t="s">
         <v>175</v>
       </c>
-      <c r="G24" s="216"/>
-      <c r="H24" s="215" t="s">
+      <c r="G24" s="239"/>
+      <c r="H24" s="236" t="s">
         <v>116</v>
       </c>
-      <c r="I24" s="216"/>
+      <c r="I24" s="239"/>
       <c r="J24" s="59" t="s">
         <v>12</v>
       </c>
@@ -6576,11 +6571,11 @@
       <c r="AB24" s="3"/>
     </row>
     <row r="25" spans="1:28" ht="81" customHeight="1" thickBot="1">
-      <c r="A25" s="192"/>
+      <c r="A25" s="256"/>
       <c r="B25" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="227"/>
+      <c r="C25" s="323"/>
       <c r="D25" s="51"/>
       <c r="E25" s="51" t="s">
         <v>219</v>
@@ -6588,14 +6583,14 @@
       <c r="F25" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="219" t="s">
+      <c r="G25" s="227" t="s">
         <v>246</v>
       </c>
-      <c r="H25" s="220"/>
-      <c r="I25" s="221" t="s">
+      <c r="H25" s="349"/>
+      <c r="I25" s="350" t="s">
         <v>248</v>
       </c>
-      <c r="J25" s="222"/>
+      <c r="J25" s="245"/>
       <c r="K25" s="7"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -6616,27 +6611,27 @@
       <c r="AB25" s="3"/>
     </row>
     <row r="26" spans="1:28" ht="47.25">
-      <c r="A26" s="192"/>
+      <c r="A26" s="256"/>
       <c r="B26" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="194" t="s">
+      <c r="C26" s="338" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="228" t="s">
+      <c r="D26" s="333" t="s">
         <v>194</v>
       </c>
-      <c r="E26" s="216"/>
+      <c r="E26" s="239"/>
       <c r="F26" s="69" t="s">
         <v>64</v>
       </c>
       <c r="G26" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="219" t="s">
+      <c r="H26" s="227" t="s">
         <v>73</v>
       </c>
-      <c r="I26" s="216"/>
+      <c r="I26" s="239"/>
       <c r="J26" s="61"/>
       <c r="K26" s="6"/>
       <c r="L26" s="2"/>
@@ -6658,11 +6653,11 @@
       <c r="AB26" s="3"/>
     </row>
     <row r="27" spans="1:28" ht="47.25">
-      <c r="A27" s="192"/>
+      <c r="A27" s="256"/>
       <c r="B27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="195"/>
+      <c r="C27" s="296"/>
       <c r="D27" s="51" t="s">
         <v>184</v>
       </c>
@@ -6675,10 +6670,10 @@
       <c r="G27" s="151" t="s">
         <v>172</v>
       </c>
-      <c r="H27" s="229" t="s">
+      <c r="H27" s="279" t="s">
         <v>143</v>
       </c>
-      <c r="I27" s="216"/>
+      <c r="I27" s="239"/>
       <c r="J27" s="64" t="s">
         <v>190</v>
       </c>
@@ -6702,25 +6697,25 @@
       <c r="AB27" s="3"/>
     </row>
     <row r="28" spans="1:28" ht="63">
-      <c r="A28" s="192"/>
+      <c r="A28" s="256"/>
       <c r="B28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="195"/>
+      <c r="C28" s="296"/>
       <c r="D28" s="105" t="s">
         <v>221</v>
       </c>
       <c r="E28" s="70" t="s">
         <v>187</v>
       </c>
-      <c r="F28" s="208" t="s">
+      <c r="F28" s="302" t="s">
         <v>213</v>
       </c>
-      <c r="G28" s="209"/>
-      <c r="H28" s="219" t="s">
+      <c r="G28" s="343"/>
+      <c r="H28" s="227" t="s">
         <v>74</v>
       </c>
-      <c r="I28" s="216"/>
+      <c r="I28" s="239"/>
       <c r="J28" s="90"/>
       <c r="K28" s="6"/>
       <c r="L28" s="2"/>
@@ -6742,11 +6737,11 @@
       <c r="AB28" s="3"/>
     </row>
     <row r="29" spans="1:28" ht="62.25" customHeight="1">
-      <c r="A29" s="192"/>
+      <c r="A29" s="256"/>
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="195"/>
+      <c r="C29" s="296"/>
       <c r="D29" s="23" t="s">
         <v>61</v>
       </c>
@@ -6788,26 +6783,26 @@
       <c r="AB29" s="3"/>
     </row>
     <row r="30" spans="1:28" ht="63">
-      <c r="A30" s="192"/>
+      <c r="A30" s="256"/>
       <c r="B30" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="195"/>
-      <c r="D30" s="217" t="s">
+      <c r="C30" s="296"/>
+      <c r="D30" s="348" t="s">
         <v>234</v>
       </c>
-      <c r="E30" s="218"/>
-      <c r="F30" s="230" t="s">
+      <c r="E30" s="252"/>
+      <c r="F30" s="334" t="s">
         <v>188</v>
       </c>
-      <c r="G30" s="216"/>
+      <c r="G30" s="239"/>
       <c r="H30" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="219" t="s">
+      <c r="I30" s="227" t="s">
         <v>244</v>
       </c>
-      <c r="J30" s="207"/>
+      <c r="J30" s="233"/>
       <c r="K30" s="6"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -6828,19 +6823,19 @@
       <c r="AB30" s="3"/>
     </row>
     <row r="31" spans="1:28" ht="60.75" customHeight="1">
-      <c r="A31" s="192"/>
+      <c r="A31" s="256"/>
       <c r="B31" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="195"/>
+      <c r="C31" s="296"/>
       <c r="D31" s="134"/>
       <c r="E31" s="135"/>
       <c r="F31" s="136"/>
       <c r="G31" s="137"/>
-      <c r="H31" s="217" t="s">
+      <c r="H31" s="348" t="s">
         <v>226</v>
       </c>
-      <c r="I31" s="225"/>
+      <c r="I31" s="267"/>
       <c r="J31" s="61"/>
       <c r="K31" s="6"/>
       <c r="L31" s="2"/>
@@ -6862,11 +6857,11 @@
       <c r="AB31" s="3"/>
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
-      <c r="A32" s="192"/>
+      <c r="A32" s="256"/>
       <c r="B32" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="196"/>
+      <c r="C32" s="322"/>
       <c r="D32" s="125"/>
       <c r="E32" s="125"/>
       <c r="F32" s="125"/>
@@ -6894,11 +6889,11 @@
       <c r="AB32" s="3"/>
     </row>
     <row r="33" spans="1:28" ht="54.75" customHeight="1">
-      <c r="A33" s="192"/>
+      <c r="A33" s="256"/>
       <c r="B33" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="197"/>
+      <c r="C33" s="339"/>
       <c r="D33" s="125"/>
       <c r="E33" s="125"/>
       <c r="F33" s="125"/>
@@ -6926,25 +6921,25 @@
       <c r="AB33" s="3"/>
     </row>
     <row r="34" spans="1:28" ht="49.5">
-      <c r="A34" s="192"/>
+      <c r="A34" s="256"/>
       <c r="B34" s="18" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="208" t="s">
+      <c r="D34" s="302" t="s">
         <v>201</v>
       </c>
-      <c r="E34" s="210"/>
-      <c r="F34" s="208" t="s">
+      <c r="E34" s="240"/>
+      <c r="F34" s="302" t="s">
         <v>111</v>
       </c>
-      <c r="G34" s="210"/>
-      <c r="H34" s="208" t="s">
+      <c r="G34" s="240"/>
+      <c r="H34" s="302" t="s">
         <v>222</v>
       </c>
-      <c r="I34" s="210"/>
+      <c r="I34" s="240"/>
       <c r="J34" s="93"/>
       <c r="K34" s="6"/>
       <c r="L34" s="2"/>
@@ -6966,19 +6961,19 @@
       <c r="AB34" s="3"/>
     </row>
     <row r="35" spans="1:28" ht="53.25" thickBot="1">
-      <c r="A35" s="193"/>
+      <c r="A35" s="257"/>
       <c r="B35" s="78" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="141" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="198" t="s">
+      <c r="D35" s="340" t="s">
         <v>251</v>
       </c>
-      <c r="E35" s="199"/>
-      <c r="F35" s="200"/>
-      <c r="G35" s="201"/>
+      <c r="E35" s="341"/>
+      <c r="F35" s="277"/>
+      <c r="G35" s="284"/>
       <c r="H35" s="84" t="s">
         <v>233</v>
       </c>
@@ -7005,10 +7000,10 @@
     </row>
     <row r="36" spans="1:28" ht="20.25" thickBot="1">
       <c r="A36" s="45"/>
-      <c r="B36" s="280" t="s">
+      <c r="B36" s="285" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="244"/>
+      <c r="C36" s="286"/>
       <c r="D36" s="27"/>
       <c r="E36" s="42"/>
       <c r="F36" s="42"/>
@@ -7036,7 +7031,7 @@
       <c r="AB36" s="3"/>
     </row>
     <row r="37" spans="1:28" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A37" s="268" t="s">
+      <c r="A37" s="295" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="53" t="s">
@@ -7084,11 +7079,11 @@
       <c r="AB37" s="3"/>
     </row>
     <row r="38" spans="1:28" ht="52.5" customHeight="1">
-      <c r="A38" s="195"/>
+      <c r="A38" s="296"/>
       <c r="B38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="281" t="s">
+      <c r="C38" s="287" t="s">
         <v>30</v>
       </c>
       <c r="D38" s="22" t="s">
@@ -7097,14 +7092,14 @@
       <c r="E38" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="219" t="s">
+      <c r="F38" s="227" t="s">
         <v>140</v>
       </c>
-      <c r="G38" s="216"/>
-      <c r="H38" s="215" t="s">
+      <c r="G38" s="239"/>
+      <c r="H38" s="236" t="s">
         <v>173</v>
       </c>
-      <c r="I38" s="216"/>
+      <c r="I38" s="239"/>
       <c r="J38" s="59" t="s">
         <v>12</v>
       </c>
@@ -7128,23 +7123,23 @@
       <c r="AB38" s="3"/>
     </row>
     <row r="39" spans="1:28" ht="58.5" customHeight="1">
-      <c r="A39" s="195"/>
+      <c r="A39" s="296"/>
       <c r="B39" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="282"/>
-      <c r="D39" s="215" t="s">
+      <c r="C39" s="269"/>
+      <c r="D39" s="236" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="210"/>
-      <c r="F39" s="265" t="s">
+      <c r="E39" s="240"/>
+      <c r="F39" s="238" t="s">
         <v>216</v>
       </c>
-      <c r="G39" s="216"/>
-      <c r="H39" s="219" t="s">
+      <c r="G39" s="239"/>
+      <c r="H39" s="227" t="s">
         <v>139</v>
       </c>
-      <c r="I39" s="216"/>
+      <c r="I39" s="239"/>
       <c r="J39" s="59" t="s">
         <v>12</v>
       </c>
@@ -7168,15 +7163,15 @@
       <c r="AB39" s="3"/>
     </row>
     <row r="40" spans="1:28" ht="57" customHeight="1">
-      <c r="A40" s="195"/>
+      <c r="A40" s="296"/>
       <c r="B40" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="283"/>
-      <c r="D40" s="215" t="s">
+      <c r="C40" s="288"/>
+      <c r="D40" s="236" t="s">
         <v>123</v>
       </c>
-      <c r="E40" s="203"/>
+      <c r="E40" s="301"/>
       <c r="F40" s="125"/>
       <c r="G40" s="89"/>
       <c r="H40" s="22" t="s">
@@ -7208,26 +7203,26 @@
       <c r="AB40" s="3"/>
     </row>
     <row r="41" spans="1:28" ht="55.5" customHeight="1">
-      <c r="A41" s="195"/>
+      <c r="A41" s="296"/>
       <c r="B41" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="284" t="s">
+      <c r="C41" s="289" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="215" t="s">
+      <c r="D41" s="236" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="257"/>
-      <c r="F41" s="312" t="s">
+      <c r="E41" s="237"/>
+      <c r="F41" s="251" t="s">
         <v>76</v>
       </c>
-      <c r="G41" s="218"/>
+      <c r="G41" s="252"/>
       <c r="H41" s="23"/>
-      <c r="I41" s="219" t="s">
+      <c r="I41" s="227" t="s">
         <v>91</v>
       </c>
-      <c r="J41" s="222"/>
+      <c r="J41" s="245"/>
       <c r="K41" s="6"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
@@ -7248,15 +7243,15 @@
       <c r="AB41" s="3"/>
     </row>
     <row r="42" spans="1:28" ht="64.5" customHeight="1">
-      <c r="A42" s="195"/>
+      <c r="A42" s="296"/>
       <c r="B42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="282"/>
-      <c r="D42" s="215" t="s">
+      <c r="C42" s="269"/>
+      <c r="D42" s="236" t="s">
         <v>168</v>
       </c>
-      <c r="E42" s="203"/>
+      <c r="E42" s="301"/>
       <c r="F42" s="154" t="s">
         <v>78</v>
       </c>
@@ -7292,22 +7287,22 @@
       <c r="AB42" s="3"/>
     </row>
     <row r="43" spans="1:28" ht="108.75" customHeight="1">
-      <c r="A43" s="195"/>
+      <c r="A43" s="296"/>
       <c r="B43" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="282"/>
-      <c r="D43" s="219" t="s">
+      <c r="C43" s="269"/>
+      <c r="D43" s="227" t="s">
         <v>232</v>
       </c>
-      <c r="E43" s="257"/>
+      <c r="E43" s="237"/>
       <c r="F43" s="144" t="s">
         <v>214</v>
       </c>
-      <c r="G43" s="208" t="s">
+      <c r="G43" s="302" t="s">
         <v>260</v>
       </c>
-      <c r="H43" s="216"/>
+      <c r="H43" s="239"/>
       <c r="I43" s="89"/>
       <c r="J43" s="90"/>
       <c r="K43" s="6"/>
@@ -7330,22 +7325,22 @@
       <c r="AB43" s="3"/>
     </row>
     <row r="44" spans="1:28" ht="63" customHeight="1">
-      <c r="A44" s="195"/>
+      <c r="A44" s="296"/>
       <c r="B44" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="282"/>
-      <c r="D44" s="215" t="s">
+      <c r="C44" s="269"/>
+      <c r="D44" s="236" t="s">
         <v>186</v>
       </c>
-      <c r="E44" s="257"/>
+      <c r="E44" s="237"/>
       <c r="F44" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="G44" s="215" t="s">
+      <c r="G44" s="236" t="s">
         <v>93</v>
       </c>
-      <c r="H44" s="216"/>
+      <c r="H44" s="239"/>
       <c r="I44" s="26"/>
       <c r="J44" s="61"/>
       <c r="K44" s="6"/>
@@ -7368,13 +7363,13 @@
       <c r="AB44" s="3"/>
     </row>
     <row r="45" spans="1:28" ht="64.5" hidden="1" customHeight="1">
-      <c r="A45" s="195"/>
+      <c r="A45" s="296"/>
       <c r="B45" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="282"/>
-      <c r="D45" s="273"/>
-      <c r="E45" s="216"/>
+      <c r="C45" s="269"/>
+      <c r="D45" s="303"/>
+      <c r="E45" s="239"/>
       <c r="F45" s="26"/>
       <c r="G45" s="39"/>
       <c r="H45" s="26"/>
@@ -7400,11 +7395,11 @@
       <c r="AB45" s="3"/>
     </row>
     <row r="46" spans="1:28" ht="47.25">
-      <c r="A46" s="195"/>
+      <c r="A46" s="296"/>
       <c r="B46" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="282"/>
+      <c r="C46" s="269"/>
       <c r="D46" s="66" t="s">
         <v>79</v>
       </c>
@@ -7417,10 +7412,10 @@
       <c r="G46" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="H46" s="215" t="s">
+      <c r="H46" s="236" t="s">
         <v>166</v>
       </c>
-      <c r="I46" s="216"/>
+      <c r="I46" s="239"/>
       <c r="J46" s="64" t="s">
         <v>32</v>
       </c>
@@ -7444,19 +7439,19 @@
       <c r="AB46" s="3"/>
     </row>
     <row r="47" spans="1:28" ht="50.25" customHeight="1">
-      <c r="A47" s="195"/>
+      <c r="A47" s="296"/>
       <c r="B47" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="282"/>
+      <c r="C47" s="269"/>
       <c r="D47" s="134"/>
       <c r="E47" s="135"/>
       <c r="F47" s="136"/>
       <c r="G47" s="137"/>
-      <c r="H47" s="265" t="s">
+      <c r="H47" s="238" t="s">
         <v>167</v>
       </c>
-      <c r="I47" s="225"/>
+      <c r="I47" s="267"/>
       <c r="J47" s="60"/>
       <c r="K47" s="6"/>
       <c r="L47" s="2"/>
@@ -7478,11 +7473,11 @@
       <c r="AB47" s="3"/>
     </row>
     <row r="48" spans="1:28" ht="49.5" customHeight="1">
-      <c r="A48" s="195"/>
+      <c r="A48" s="296"/>
       <c r="B48" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="285"/>
+      <c r="C48" s="290"/>
       <c r="D48" s="125"/>
       <c r="E48" s="125"/>
       <c r="F48" s="125"/>
@@ -7510,15 +7505,15 @@
       <c r="AB48" s="3"/>
     </row>
     <row r="49" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A49" s="195"/>
+      <c r="A49" s="296"/>
       <c r="B49" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C49" s="286"/>
-      <c r="D49" s="204" t="s">
+      <c r="C49" s="291"/>
+      <c r="D49" s="253" t="s">
         <v>115</v>
       </c>
-      <c r="E49" s="205"/>
+      <c r="E49" s="242"/>
       <c r="F49" s="125"/>
       <c r="G49" s="125"/>
       <c r="H49" s="125"/>
@@ -7544,7 +7539,7 @@
       <c r="AB49" s="3"/>
     </row>
     <row r="50" spans="1:28" ht="49.5">
-      <c r="A50" s="195"/>
+      <c r="A50" s="296"/>
       <c r="B50" s="19" t="s">
         <v>25</v>
       </c>
@@ -7555,14 +7550,14 @@
         <v>181</v>
       </c>
       <c r="E50" s="145"/>
-      <c r="F50" s="259" t="s">
+      <c r="F50" s="241" t="s">
         <v>236</v>
       </c>
-      <c r="G50" s="205"/>
-      <c r="H50" s="259" t="s">
+      <c r="G50" s="242"/>
+      <c r="H50" s="241" t="s">
         <v>210</v>
       </c>
-      <c r="I50" s="205"/>
+      <c r="I50" s="242"/>
       <c r="J50" s="122"/>
       <c r="K50" s="8"/>
       <c r="L50" s="2"/>
@@ -7584,7 +7579,7 @@
       <c r="AB50" s="3"/>
     </row>
     <row r="51" spans="1:28" ht="79.5" thickBot="1">
-      <c r="A51" s="269"/>
+      <c r="A51" s="297"/>
       <c r="B51" s="62" t="s">
         <v>26</v>
       </c>
@@ -7597,14 +7592,14 @@
       <c r="E51" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="F51" s="308" t="s">
+      <c r="F51" s="246" t="s">
         <v>238</v>
       </c>
-      <c r="G51" s="309"/>
-      <c r="H51" s="262" t="s">
+      <c r="G51" s="247"/>
+      <c r="H51" s="293" t="s">
         <v>162</v>
       </c>
-      <c r="I51" s="263"/>
+      <c r="I51" s="294"/>
       <c r="J51" s="85" t="s">
         <v>163</v>
       </c>
@@ -7629,10 +7624,10 @@
     </row>
     <row r="52" spans="1:28" ht="21.75" customHeight="1" thickBot="1">
       <c r="A52" s="46"/>
-      <c r="B52" s="287" t="s">
+      <c r="B52" s="292" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="224"/>
+      <c r="C52" s="262"/>
       <c r="D52" s="27"/>
       <c r="E52" s="28"/>
       <c r="F52" s="28"/>
@@ -7660,7 +7655,7 @@
       <c r="AB52" s="3"/>
     </row>
     <row r="53" spans="1:28" ht="19.5">
-      <c r="A53" s="270" t="s">
+      <c r="A53" s="298" t="s">
         <v>33</v>
       </c>
       <c r="B53" s="160" t="s">
@@ -7708,25 +7703,25 @@
       <c r="AB53" s="3"/>
     </row>
     <row r="54" spans="1:28" ht="56.25" customHeight="1">
-      <c r="A54" s="271"/>
+      <c r="A54" s="299"/>
       <c r="B54" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="290" t="s">
+      <c r="C54" s="258" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="204" t="s">
+      <c r="D54" s="253" t="s">
         <v>178</v>
       </c>
-      <c r="E54" s="205"/>
-      <c r="F54" s="204" t="s">
+      <c r="E54" s="242"/>
+      <c r="F54" s="253" t="s">
         <v>176</v>
       </c>
-      <c r="G54" s="205"/>
-      <c r="H54" s="204" t="s">
+      <c r="G54" s="242"/>
+      <c r="H54" s="253" t="s">
         <v>218</v>
       </c>
-      <c r="I54" s="205"/>
+      <c r="I54" s="242"/>
       <c r="J54" s="164" t="s">
         <v>12</v>
       </c>
@@ -7750,24 +7745,24 @@
       <c r="AB54" s="3"/>
     </row>
     <row r="55" spans="1:28" ht="60" customHeight="1">
-      <c r="A55" s="271"/>
+      <c r="A55" s="299"/>
       <c r="B55" s="155" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="205"/>
-      <c r="D55" s="204" t="s">
+      <c r="C55" s="242"/>
+      <c r="D55" s="253" t="s">
         <v>154</v>
       </c>
-      <c r="E55" s="205"/>
-      <c r="F55" s="204" t="s">
+      <c r="E55" s="242"/>
+      <c r="F55" s="253" t="s">
         <v>155</v>
       </c>
-      <c r="G55" s="205"/>
+      <c r="G55" s="242"/>
       <c r="H55" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="I55" s="304"/>
-      <c r="J55" s="305"/>
+      <c r="I55" s="234"/>
+      <c r="J55" s="235"/>
       <c r="K55" s="5"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
@@ -7788,28 +7783,28 @@
       <c r="AB55" s="3"/>
     </row>
     <row r="56" spans="1:28" ht="78" customHeight="1">
-      <c r="A56" s="271"/>
+      <c r="A56" s="299"/>
       <c r="B56" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="205"/>
+      <c r="C56" s="242"/>
       <c r="D56" s="156" t="s">
         <v>12</v>
       </c>
       <c r="E56" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="F56" s="259" t="s">
+      <c r="F56" s="241" t="s">
         <v>142</v>
       </c>
-      <c r="G56" s="205"/>
+      <c r="G56" s="242"/>
       <c r="H56" s="151" t="s">
         <v>83</v>
       </c>
-      <c r="I56" s="204" t="s">
+      <c r="I56" s="253" t="s">
         <v>164</v>
       </c>
-      <c r="J56" s="267"/>
+      <c r="J56" s="254"/>
       <c r="K56" s="6"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
@@ -7830,21 +7825,21 @@
       <c r="AB56" s="3"/>
     </row>
     <row r="57" spans="1:28" ht="47.25">
-      <c r="A57" s="271"/>
+      <c r="A57" s="299"/>
       <c r="B57" s="155" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="291" t="s">
+      <c r="C57" s="259" t="s">
         <v>16</v>
       </c>
-      <c r="D57" s="306" t="s">
+      <c r="D57" s="243" t="s">
         <v>249</v>
       </c>
-      <c r="E57" s="307"/>
-      <c r="F57" s="310" t="s">
+      <c r="E57" s="244"/>
+      <c r="F57" s="248" t="s">
         <v>240</v>
       </c>
-      <c r="G57" s="310"/>
+      <c r="G57" s="248"/>
       <c r="H57" s="151" t="s">
         <v>81</v>
       </c>
@@ -7872,11 +7867,11 @@
       <c r="AB57" s="3"/>
     </row>
     <row r="58" spans="1:28" ht="60" customHeight="1">
-      <c r="A58" s="271"/>
+      <c r="A58" s="299"/>
       <c r="B58" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="205"/>
+      <c r="C58" s="242"/>
       <c r="D58" s="157" t="s">
         <v>149</v>
       </c>
@@ -7889,10 +7884,10 @@
       <c r="G58" s="151" t="s">
         <v>237</v>
       </c>
-      <c r="H58" s="259" t="s">
+      <c r="H58" s="241" t="s">
         <v>77</v>
       </c>
-      <c r="I58" s="259"/>
+      <c r="I58" s="241"/>
       <c r="J58" s="166"/>
       <c r="K58" s="5"/>
       <c r="L58" s="2"/>
@@ -7914,15 +7909,15 @@
       <c r="AB58" s="3"/>
     </row>
     <row r="59" spans="1:28" ht="54" customHeight="1">
-      <c r="A59" s="271"/>
+      <c r="A59" s="299"/>
       <c r="B59" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="205"/>
-      <c r="D59" s="204" t="s">
+      <c r="C59" s="242"/>
+      <c r="D59" s="253" t="s">
         <v>84</v>
       </c>
-      <c r="E59" s="205"/>
+      <c r="E59" s="242"/>
       <c r="F59" s="151" t="s">
         <v>225</v>
       </c>
@@ -7956,15 +7951,15 @@
       <c r="AB59" s="3"/>
     </row>
     <row r="60" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A60" s="271"/>
+      <c r="A60" s="299"/>
       <c r="B60" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="205"/>
-      <c r="D60" s="204" t="s">
+      <c r="C60" s="242"/>
+      <c r="D60" s="253" t="s">
         <v>95</v>
       </c>
-      <c r="E60" s="205"/>
+      <c r="E60" s="242"/>
       <c r="F60" s="150" t="s">
         <v>97</v>
       </c>
@@ -7998,11 +7993,11 @@
       <c r="AB60" s="3"/>
     </row>
     <row r="61" spans="1:28" ht="47.25">
-      <c r="A61" s="271"/>
+      <c r="A61" s="299"/>
       <c r="B61" s="155" t="s">
         <v>21</v>
       </c>
-      <c r="C61" s="205"/>
+      <c r="C61" s="242"/>
       <c r="D61" s="125"/>
       <c r="E61" s="125"/>
       <c r="F61" s="157" t="s">
@@ -8014,10 +8009,10 @@
       <c r="H61" s="150" t="s">
         <v>183</v>
       </c>
-      <c r="I61" s="259" t="s">
+      <c r="I61" s="241" t="s">
         <v>245</v>
       </c>
-      <c r="J61" s="267"/>
+      <c r="J61" s="254"/>
       <c r="K61" s="5"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
@@ -8038,21 +8033,21 @@
       <c r="AB61" s="3"/>
     </row>
     <row r="62" spans="1:28" ht="47.25" customHeight="1">
-      <c r="A62" s="271"/>
+      <c r="A62" s="299"/>
       <c r="B62" s="155" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="205"/>
+      <c r="C62" s="242"/>
       <c r="D62" s="158"/>
       <c r="E62" s="158"/>
-      <c r="F62" s="204" t="s">
+      <c r="F62" s="253" t="s">
         <v>165</v>
       </c>
-      <c r="G62" s="205"/>
-      <c r="H62" s="274" t="s">
+      <c r="G62" s="242"/>
+      <c r="H62" s="304" t="s">
         <v>169</v>
       </c>
-      <c r="I62" s="275"/>
+      <c r="I62" s="305"/>
       <c r="J62" s="167"/>
       <c r="K62" s="5"/>
       <c r="L62" s="2"/>
@@ -8074,11 +8069,11 @@
       <c r="AB62" s="3"/>
     </row>
     <row r="63" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A63" s="271"/>
+      <c r="A63" s="299"/>
       <c r="B63" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="292" t="s">
+      <c r="C63" s="260" t="s">
         <v>16</v>
       </c>
       <c r="D63" s="125"/>
@@ -8108,19 +8103,19 @@
       <c r="AB63" s="3"/>
     </row>
     <row r="64" spans="1:28" ht="51" customHeight="1">
-      <c r="A64" s="271"/>
+      <c r="A64" s="299"/>
       <c r="B64" s="155" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="205"/>
+      <c r="C64" s="242"/>
       <c r="D64" s="125"/>
       <c r="E64" s="125"/>
       <c r="F64" s="125"/>
       <c r="G64" s="125"/>
-      <c r="H64" s="204" t="s">
+      <c r="H64" s="253" t="s">
         <v>179</v>
       </c>
-      <c r="I64" s="205"/>
+      <c r="I64" s="242"/>
       <c r="J64" s="167"/>
       <c r="K64" s="5"/>
       <c r="L64" s="2"/>
@@ -8142,7 +8137,7 @@
       <c r="AB64" s="3"/>
     </row>
     <row r="65" spans="1:28" ht="50.25" customHeight="1">
-      <c r="A65" s="271"/>
+      <c r="A65" s="299"/>
       <c r="B65" s="155" t="s">
         <v>25</v>
       </c>
@@ -8155,14 +8150,14 @@
       <c r="E65" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="F65" s="204" t="s">
+      <c r="F65" s="253" t="s">
         <v>170</v>
       </c>
-      <c r="G65" s="205"/>
-      <c r="H65" s="204" t="s">
+      <c r="G65" s="242"/>
+      <c r="H65" s="253" t="s">
         <v>217</v>
       </c>
-      <c r="I65" s="205"/>
+      <c r="I65" s="242"/>
       <c r="J65" s="166"/>
       <c r="K65" s="5"/>
       <c r="L65" s="2"/>
@@ -8184,7 +8179,7 @@
       <c r="AB65" s="3"/>
     </row>
     <row r="66" spans="1:28" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A66" s="272"/>
+      <c r="A66" s="300"/>
       <c r="B66" s="168" t="s">
         <v>26</v>
       </c>
@@ -8203,8 +8198,8 @@
       <c r="G66" s="173" t="s">
         <v>78</v>
       </c>
-      <c r="H66" s="276"/>
-      <c r="I66" s="277"/>
+      <c r="H66" s="306"/>
+      <c r="I66" s="307"/>
       <c r="J66" s="172"/>
       <c r="K66" s="5"/>
       <c r="L66" s="2"/>
@@ -8227,10 +8222,10 @@
     </row>
     <row r="67" spans="1:28" ht="20.25" thickBot="1">
       <c r="A67" s="46"/>
-      <c r="B67" s="293" t="s">
+      <c r="B67" s="261" t="s">
         <v>35</v>
       </c>
-      <c r="C67" s="224"/>
+      <c r="C67" s="262"/>
       <c r="D67" s="27"/>
       <c r="E67" s="32"/>
       <c r="F67" s="32"/>
@@ -8258,7 +8253,7 @@
       <c r="AB67" s="3"/>
     </row>
     <row r="68" spans="1:28" ht="61.5" customHeight="1" thickBot="1">
-      <c r="A68" s="289" t="s">
+      <c r="A68" s="255" t="s">
         <v>36</v>
       </c>
       <c r="B68" s="71" t="s">
@@ -8304,11 +8299,11 @@
       <c r="AB68" s="3"/>
     </row>
     <row r="69" spans="1:28" ht="64.5" customHeight="1">
-      <c r="A69" s="192"/>
+      <c r="A69" s="256"/>
       <c r="B69" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="258" t="s">
+      <c r="C69" s="263" t="s">
         <v>43</v>
       </c>
       <c r="D69" s="47" t="s">
@@ -8323,7 +8318,7 @@
       <c r="G69" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="295" t="s">
+      <c r="H69" s="268" t="s">
         <v>185</v>
       </c>
       <c r="I69" s="22" t="s">
@@ -8352,26 +8347,26 @@
       <c r="AB69" s="3"/>
     </row>
     <row r="70" spans="1:28" ht="50.25" customHeight="1">
-      <c r="A70" s="192"/>
+      <c r="A70" s="256"/>
       <c r="B70" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="252"/>
+      <c r="C70" s="264"/>
       <c r="D70" s="47" t="s">
         <v>12</v>
       </c>
       <c r="E70" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="215" t="s">
+      <c r="F70" s="236" t="s">
         <v>96</v>
       </c>
-      <c r="G70" s="257"/>
-      <c r="H70" s="282"/>
-      <c r="I70" s="232" t="s">
+      <c r="G70" s="237"/>
+      <c r="H70" s="269"/>
+      <c r="I70" s="249" t="s">
         <v>241</v>
       </c>
-      <c r="J70" s="311"/>
+      <c r="J70" s="250"/>
       <c r="K70" s="6"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
@@ -8392,24 +8387,24 @@
       <c r="AB70" s="3"/>
     </row>
     <row r="71" spans="1:28" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A71" s="192"/>
+      <c r="A71" s="256"/>
       <c r="B71" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C71" s="253"/>
-      <c r="D71" s="297" t="s">
+      <c r="C71" s="265"/>
+      <c r="D71" s="271" t="s">
         <v>202</v>
       </c>
-      <c r="E71" s="298"/>
+      <c r="E71" s="272"/>
       <c r="F71" s="121"/>
       <c r="G71" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="H71" s="282"/>
-      <c r="I71" s="288" t="s">
+      <c r="H71" s="269"/>
+      <c r="I71" s="232" t="s">
         <v>203</v>
       </c>
-      <c r="J71" s="207"/>
+      <c r="J71" s="233"/>
       <c r="K71" s="6"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
@@ -8430,26 +8425,26 @@
       <c r="AB71" s="3"/>
     </row>
     <row r="72" spans="1:28" ht="52.5" customHeight="1">
-      <c r="A72" s="192"/>
+      <c r="A72" s="256"/>
       <c r="B72" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C72" s="294" t="s">
+      <c r="C72" s="266" t="s">
         <v>16</v>
       </c>
-      <c r="D72" s="297" t="s">
+      <c r="D72" s="271" t="s">
         <v>86</v>
       </c>
-      <c r="E72" s="298"/>
-      <c r="F72" s="215" t="s">
+      <c r="E72" s="272"/>
+      <c r="F72" s="236" t="s">
         <v>192</v>
       </c>
-      <c r="G72" s="207"/>
-      <c r="H72" s="282"/>
-      <c r="I72" s="288" t="s">
+      <c r="G72" s="233"/>
+      <c r="H72" s="269"/>
+      <c r="I72" s="232" t="s">
         <v>87</v>
       </c>
-      <c r="J72" s="207"/>
+      <c r="J72" s="233"/>
       <c r="K72" s="6"/>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
@@ -8470,26 +8465,26 @@
       <c r="AB72" s="3"/>
     </row>
     <row r="73" spans="1:28" ht="61.5" customHeight="1">
-      <c r="A73" s="192"/>
+      <c r="A73" s="256"/>
       <c r="B73" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C73" s="252"/>
+      <c r="C73" s="264"/>
       <c r="D73" s="88" t="s">
         <v>153</v>
       </c>
       <c r="E73" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="F73" s="299" t="s">
+      <c r="F73" s="273" t="s">
         <v>253</v>
       </c>
-      <c r="G73" s="300"/>
-      <c r="H73" s="282"/>
-      <c r="I73" s="299" t="s">
+      <c r="G73" s="274"/>
+      <c r="H73" s="269"/>
+      <c r="I73" s="273" t="s">
         <v>254</v>
       </c>
-      <c r="J73" s="301"/>
+      <c r="J73" s="275"/>
       <c r="K73" s="6"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
@@ -8510,24 +8505,24 @@
       <c r="AB73" s="3"/>
     </row>
     <row r="74" spans="1:28" ht="60.75" customHeight="1">
-      <c r="A74" s="192"/>
+      <c r="A74" s="256"/>
       <c r="B74" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C74" s="252"/>
-      <c r="D74" s="229" t="s">
+      <c r="C74" s="264"/>
+      <c r="D74" s="279" t="s">
         <v>180</v>
       </c>
-      <c r="E74" s="216"/>
-      <c r="F74" s="288" t="s">
+      <c r="E74" s="239"/>
+      <c r="F74" s="232" t="s">
         <v>125</v>
       </c>
-      <c r="G74" s="216"/>
-      <c r="H74" s="282"/>
-      <c r="I74" s="256" t="s">
+      <c r="G74" s="239"/>
+      <c r="H74" s="269"/>
+      <c r="I74" s="308" t="s">
         <v>126</v>
       </c>
-      <c r="J74" s="207"/>
+      <c r="J74" s="233"/>
       <c r="K74" s="6"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
@@ -8548,24 +8543,24 @@
       <c r="AB74" s="3"/>
     </row>
     <row r="75" spans="1:28" ht="69" customHeight="1">
-      <c r="A75" s="192"/>
+      <c r="A75" s="256"/>
       <c r="B75" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C75" s="252"/>
-      <c r="D75" s="229" t="s">
+      <c r="C75" s="264"/>
+      <c r="D75" s="279" t="s">
         <v>88</v>
       </c>
-      <c r="E75" s="216"/>
-      <c r="F75" s="202" t="s">
+      <c r="E75" s="239"/>
+      <c r="F75" s="280" t="s">
         <v>134</v>
       </c>
-      <c r="G75" s="216"/>
-      <c r="H75" s="282"/>
-      <c r="I75" s="215" t="s">
+      <c r="G75" s="239"/>
+      <c r="H75" s="269"/>
+      <c r="I75" s="236" t="s">
         <v>124</v>
       </c>
-      <c r="J75" s="207"/>
+      <c r="J75" s="233"/>
       <c r="K75" s="6"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
@@ -8586,24 +8581,24 @@
       <c r="AB75" s="3"/>
     </row>
     <row r="76" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A76" s="192"/>
+      <c r="A76" s="256"/>
       <c r="B76" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C76" s="252"/>
-      <c r="D76" s="215" t="s">
+      <c r="C76" s="264"/>
+      <c r="D76" s="236" t="s">
         <v>197</v>
       </c>
-      <c r="E76" s="257"/>
-      <c r="F76" s="202" t="s">
+      <c r="E76" s="237"/>
+      <c r="F76" s="280" t="s">
         <v>110</v>
       </c>
-      <c r="G76" s="216"/>
-      <c r="H76" s="282"/>
-      <c r="I76" s="215" t="s">
+      <c r="G76" s="239"/>
+      <c r="H76" s="269"/>
+      <c r="I76" s="236" t="s">
         <v>145</v>
       </c>
-      <c r="J76" s="207"/>
+      <c r="J76" s="233"/>
       <c r="K76" s="6"/>
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
@@ -8624,22 +8619,22 @@
       <c r="AB76" s="3"/>
     </row>
     <row r="77" spans="1:28" ht="57" customHeight="1">
-      <c r="A77" s="192"/>
+      <c r="A77" s="256"/>
       <c r="B77" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C77" s="252"/>
-      <c r="D77" s="219" t="s">
+      <c r="C77" s="264"/>
+      <c r="D77" s="227" t="s">
         <v>243</v>
       </c>
-      <c r="E77" s="257"/>
+      <c r="E77" s="237"/>
       <c r="F77" s="25"/>
       <c r="G77" s="25"/>
-      <c r="H77" s="282"/>
-      <c r="I77" s="219" t="s">
+      <c r="H77" s="269"/>
+      <c r="I77" s="227" t="s">
         <v>242</v>
       </c>
-      <c r="J77" s="207"/>
+      <c r="J77" s="233"/>
       <c r="K77" s="11"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
@@ -8660,24 +8655,24 @@
       <c r="AB77" s="3"/>
     </row>
     <row r="78" spans="1:28" ht="55.5" customHeight="1">
-      <c r="A78" s="192"/>
+      <c r="A78" s="256"/>
       <c r="B78" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C78" s="252"/>
-      <c r="D78" s="229" t="s">
+      <c r="C78" s="264"/>
+      <c r="D78" s="279" t="s">
         <v>89</v>
       </c>
-      <c r="E78" s="216"/>
-      <c r="F78" s="215" t="s">
+      <c r="E78" s="239"/>
+      <c r="F78" s="236" t="s">
         <v>209</v>
       </c>
-      <c r="G78" s="216"/>
-      <c r="H78" s="282"/>
-      <c r="I78" s="215" t="s">
+      <c r="G78" s="239"/>
+      <c r="H78" s="269"/>
+      <c r="I78" s="236" t="s">
         <v>211</v>
       </c>
-      <c r="J78" s="207"/>
+      <c r="J78" s="233"/>
       <c r="K78" s="6"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
@@ -8698,16 +8693,16 @@
       <c r="AB78" s="3"/>
     </row>
     <row r="79" spans="1:28" ht="64.5" hidden="1" customHeight="1">
-      <c r="A79" s="192"/>
+      <c r="A79" s="256"/>
       <c r="B79" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C79" s="252"/>
+      <c r="C79" s="264"/>
       <c r="D79" s="48"/>
       <c r="E79" s="24"/>
       <c r="F79" s="24"/>
       <c r="G79" s="24"/>
-      <c r="H79" s="282"/>
+      <c r="H79" s="269"/>
       <c r="I79" s="36"/>
       <c r="J79" s="77"/>
       <c r="K79" s="6"/>
@@ -8730,24 +8725,24 @@
       <c r="AB79" s="3"/>
     </row>
     <row r="80" spans="1:28" ht="58.5" customHeight="1" thickBot="1">
-      <c r="A80" s="192"/>
+      <c r="A80" s="256"/>
       <c r="B80" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C80" s="253"/>
-      <c r="D80" s="202" t="s">
+      <c r="C80" s="265"/>
+      <c r="D80" s="280" t="s">
         <v>112</v>
       </c>
-      <c r="E80" s="216"/>
-      <c r="F80" s="278" t="s">
+      <c r="E80" s="239"/>
+      <c r="F80" s="281" t="s">
         <v>136</v>
       </c>
-      <c r="G80" s="216"/>
-      <c r="H80" s="282"/>
-      <c r="I80" s="219" t="s">
+      <c r="G80" s="239"/>
+      <c r="H80" s="269"/>
+      <c r="I80" s="227" t="s">
         <v>92</v>
       </c>
-      <c r="J80" s="207"/>
+      <c r="J80" s="233"/>
       <c r="K80" s="6"/>
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
@@ -8768,26 +8763,26 @@
       <c r="AB80" s="3"/>
     </row>
     <row r="81" spans="1:28" ht="50.25" thickBot="1">
-      <c r="A81" s="192"/>
+      <c r="A81" s="256"/>
       <c r="B81" s="18" t="s">
         <v>25</v>
       </c>
       <c r="C81" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="279" t="s">
+      <c r="D81" s="282" t="s">
         <v>117</v>
       </c>
-      <c r="E81" s="243"/>
-      <c r="F81" s="215" t="s">
+      <c r="E81" s="283"/>
+      <c r="F81" s="236" t="s">
         <v>118</v>
       </c>
-      <c r="G81" s="216"/>
-      <c r="H81" s="282"/>
-      <c r="I81" s="302" t="s">
+      <c r="G81" s="239"/>
+      <c r="H81" s="269"/>
+      <c r="I81" s="276" t="s">
         <v>224</v>
       </c>
-      <c r="J81" s="207"/>
+      <c r="J81" s="233"/>
       <c r="K81" s="6"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
@@ -8808,26 +8803,26 @@
       <c r="AB81" s="3"/>
     </row>
     <row r="82" spans="1:28" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A82" s="193"/>
+      <c r="A82" s="257"/>
       <c r="B82" s="78" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D82" s="200" t="s">
+      <c r="D82" s="277" t="s">
         <v>120</v>
       </c>
-      <c r="E82" s="201"/>
-      <c r="F82" s="200" t="s">
+      <c r="E82" s="284"/>
+      <c r="F82" s="277" t="s">
         <v>121</v>
       </c>
-      <c r="G82" s="201"/>
-      <c r="H82" s="296"/>
-      <c r="I82" s="200" t="s">
+      <c r="G82" s="284"/>
+      <c r="H82" s="270"/>
+      <c r="I82" s="277" t="s">
         <v>119</v>
       </c>
-      <c r="J82" s="303"/>
+      <c r="J82" s="278"/>
       <c r="K82" s="6"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
@@ -8848,18 +8843,18 @@
       <c r="AB82" s="3"/>
     </row>
     <row r="83" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A83" s="317"/>
-      <c r="B83" s="318" t="s">
+      <c r="A83" s="191"/>
+      <c r="B83" s="220" t="s">
         <v>50</v>
       </c>
-      <c r="C83" s="319"/>
-      <c r="D83" s="320"/>
-      <c r="E83" s="321"/>
-      <c r="F83" s="321"/>
-      <c r="G83" s="321"/>
-      <c r="H83" s="321"/>
-      <c r="I83" s="321"/>
-      <c r="J83" s="322"/>
+      <c r="C83" s="221"/>
+      <c r="D83" s="192"/>
+      <c r="E83" s="193"/>
+      <c r="F83" s="193"/>
+      <c r="G83" s="193"/>
+      <c r="H83" s="193"/>
+      <c r="I83" s="193"/>
+      <c r="J83" s="194"/>
       <c r="K83" s="1"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
@@ -8880,26 +8875,28 @@
       <c r="AB83" s="3"/>
     </row>
     <row r="84" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A84" s="323" t="s">
+      <c r="A84" s="222" t="s">
         <v>50</v>
       </c>
-      <c r="B84" s="324" t="s">
+      <c r="B84" s="195" t="s">
         <v>28</v>
       </c>
-      <c r="C84" s="324"/>
-      <c r="D84" s="325" t="s">
+      <c r="C84" s="195"/>
+      <c r="D84" s="196" t="s">
         <v>47</v>
       </c>
-      <c r="E84" s="326" t="s">
+      <c r="E84" s="197" t="s">
         <v>48</v>
       </c>
-      <c r="F84" s="327" t="s">
+      <c r="F84" s="198" t="s">
         <v>49</v>
       </c>
-      <c r="G84" s="328"/>
-      <c r="H84" s="329"/>
-      <c r="I84" s="329"/>
-      <c r="J84" s="330"/>
+      <c r="G84" s="130" t="s">
+        <v>269</v>
+      </c>
+      <c r="H84" s="200"/>
+      <c r="I84" s="200"/>
+      <c r="J84" s="201"/>
       <c r="K84" s="1"/>
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
@@ -8920,11 +8917,11 @@
       <c r="AB84" s="3"/>
     </row>
     <row r="85" spans="1:28" ht="66">
-      <c r="A85" s="331"/>
-      <c r="B85" s="332" t="s">
+      <c r="A85" s="223"/>
+      <c r="B85" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="333"/>
+      <c r="C85" s="225"/>
       <c r="D85" s="108" t="s">
         <v>204</v>
       </c>
@@ -8933,9 +8930,9 @@
       </c>
       <c r="F85" s="178"/>
       <c r="G85" s="179"/>
-      <c r="H85" s="336"/>
-      <c r="I85" s="336"/>
-      <c r="J85" s="337"/>
+      <c r="H85" s="205"/>
+      <c r="I85" s="205"/>
+      <c r="J85" s="206"/>
       <c r="K85" s="1"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
@@ -8956,11 +8953,11 @@
       <c r="AB85" s="3"/>
     </row>
     <row r="86" spans="1:28" ht="66">
-      <c r="A86" s="331"/>
-      <c r="B86" s="332" t="s">
+      <c r="A86" s="223"/>
+      <c r="B86" s="202" t="s">
         <v>17</v>
       </c>
-      <c r="C86" s="338"/>
+      <c r="C86" s="226"/>
       <c r="D86" s="109" t="s">
         <v>127</v>
       </c>
@@ -8969,9 +8966,9 @@
       </c>
       <c r="F86" s="178"/>
       <c r="G86" s="179"/>
-      <c r="H86" s="336"/>
-      <c r="I86" s="336"/>
-      <c r="J86" s="339"/>
+      <c r="H86" s="205"/>
+      <c r="I86" s="205"/>
+      <c r="J86" s="207"/>
       <c r="K86" s="1"/>
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
@@ -8992,11 +8989,11 @@
       <c r="AB86" s="3"/>
     </row>
     <row r="87" spans="1:28" ht="49.5">
-      <c r="A87" s="331"/>
-      <c r="B87" s="332" t="s">
+      <c r="A87" s="223"/>
+      <c r="B87" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="C87" s="338"/>
+      <c r="C87" s="226"/>
       <c r="D87" s="188" t="s">
         <v>257</v>
       </c>
@@ -9007,7 +9004,7 @@
       <c r="G87" s="179"/>
       <c r="H87" s="23"/>
       <c r="I87" s="23"/>
-      <c r="J87" s="339"/>
+      <c r="J87" s="207"/>
       <c r="K87" s="1"/>
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
@@ -9028,11 +9025,11 @@
       <c r="AB87" s="3"/>
     </row>
     <row r="88" spans="1:28" ht="66">
-      <c r="A88" s="331"/>
-      <c r="B88" s="332" t="s">
+      <c r="A88" s="223"/>
+      <c r="B88" s="202" t="s">
         <v>19</v>
       </c>
-      <c r="C88" s="338"/>
+      <c r="C88" s="226"/>
       <c r="D88" s="188" t="s">
         <v>256</v>
       </c>
@@ -9042,8 +9039,8 @@
       <c r="F88" s="180"/>
       <c r="G88" s="179"/>
       <c r="H88" s="23"/>
-      <c r="I88" s="340"/>
-      <c r="J88" s="339"/>
+      <c r="I88" s="208"/>
+      <c r="J88" s="207"/>
       <c r="K88" s="1"/>
       <c r="L88" s="2"/>
       <c r="M88" s="2"/>
@@ -9064,11 +9061,11 @@
       <c r="AB88" s="3"/>
     </row>
     <row r="89" spans="1:28" ht="49.5">
-      <c r="A89" s="331"/>
-      <c r="B89" s="332" t="s">
+      <c r="A89" s="223"/>
+      <c r="B89" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="C89" s="338"/>
+      <c r="C89" s="226"/>
       <c r="D89" s="109" t="s">
         <v>268</v>
       </c>
@@ -9080,8 +9077,8 @@
       </c>
       <c r="G89" s="179"/>
       <c r="H89" s="189"/>
-      <c r="I89" s="219"/>
-      <c r="J89" s="342"/>
+      <c r="I89" s="227"/>
+      <c r="J89" s="228"/>
       <c r="K89" s="1"/>
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
@@ -9102,11 +9099,11 @@
       <c r="AB89" s="3"/>
     </row>
     <row r="90" spans="1:28" ht="50.25" thickBot="1">
-      <c r="A90" s="331"/>
-      <c r="B90" s="343" t="s">
+      <c r="A90" s="223"/>
+      <c r="B90" s="210" t="s">
         <v>23</v>
       </c>
-      <c r="C90" s="344"/>
+      <c r="C90" s="211"/>
       <c r="D90" s="114"/>
       <c r="E90" s="183" t="s">
         <v>223</v>
@@ -9117,9 +9114,9 @@
       <c r="G90" s="184" t="s">
         <v>267</v>
       </c>
-      <c r="H90" s="219"/>
-      <c r="I90" s="346"/>
-      <c r="J90" s="347"/>
+      <c r="H90" s="227"/>
+      <c r="I90" s="229"/>
+      <c r="J90" s="213"/>
       <c r="K90" s="1"/>
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
@@ -9140,18 +9137,18 @@
       <c r="AB90" s="3"/>
     </row>
     <row r="91" spans="1:28" ht="32.25" thickBot="1">
-      <c r="A91" s="348"/>
-      <c r="B91" s="343" t="s">
+      <c r="A91" s="224"/>
+      <c r="B91" s="210" t="s">
         <v>24</v>
       </c>
-      <c r="C91" s="349"/>
-      <c r="D91" s="350"/>
-      <c r="E91" s="350"/>
-      <c r="F91" s="351"/>
-      <c r="G91" s="352"/>
-      <c r="H91" s="353"/>
-      <c r="I91" s="354"/>
-      <c r="J91" s="355"/>
+      <c r="C91" s="214"/>
+      <c r="D91" s="216"/>
+      <c r="E91" s="216"/>
+      <c r="F91" s="216"/>
+      <c r="G91" s="215"/>
+      <c r="H91" s="230"/>
+      <c r="I91" s="231"/>
+      <c r="J91" s="217"/>
       <c r="K91" s="1"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
@@ -9172,18 +9169,18 @@
       <c r="AB91" s="3"/>
     </row>
     <row r="92" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A92" s="317"/>
-      <c r="B92" s="318" t="s">
+      <c r="A92" s="191"/>
+      <c r="B92" s="220" t="s">
         <v>60</v>
       </c>
-      <c r="C92" s="319"/>
-      <c r="D92" s="320"/>
-      <c r="E92" s="321"/>
-      <c r="F92" s="321"/>
-      <c r="G92" s="321"/>
-      <c r="H92" s="321"/>
-      <c r="I92" s="321"/>
-      <c r="J92" s="322"/>
+      <c r="C92" s="221"/>
+      <c r="D92" s="192"/>
+      <c r="E92" s="193"/>
+      <c r="F92" s="193"/>
+      <c r="G92" s="193"/>
+      <c r="H92" s="193"/>
+      <c r="I92" s="193"/>
+      <c r="J92" s="194"/>
       <c r="K92" s="1"/>
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
@@ -9204,26 +9201,26 @@
       <c r="AB92" s="3"/>
     </row>
     <row r="93" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A93" s="323" t="s">
+      <c r="A93" s="222" t="s">
         <v>60</v>
       </c>
-      <c r="B93" s="324" t="s">
+      <c r="B93" s="195" t="s">
         <v>28</v>
       </c>
-      <c r="C93" s="324"/>
-      <c r="D93" s="325" t="s">
+      <c r="C93" s="195"/>
+      <c r="D93" s="196" t="s">
         <v>47</v>
       </c>
-      <c r="E93" s="326" t="s">
+      <c r="E93" s="197" t="s">
         <v>48</v>
       </c>
-      <c r="F93" s="327" t="s">
+      <c r="F93" s="198" t="s">
         <v>49</v>
       </c>
-      <c r="G93" s="328"/>
-      <c r="H93" s="329"/>
-      <c r="I93" s="329"/>
-      <c r="J93" s="330"/>
+      <c r="G93" s="199"/>
+      <c r="H93" s="200"/>
+      <c r="I93" s="200"/>
+      <c r="J93" s="201"/>
       <c r="K93" s="1"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
@@ -9244,11 +9241,11 @@
       <c r="AB93" s="3"/>
     </row>
     <row r="94" spans="1:28" ht="66">
-      <c r="A94" s="331"/>
-      <c r="B94" s="332" t="s">
+      <c r="A94" s="223"/>
+      <c r="B94" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="C94" s="333"/>
+      <c r="C94" s="225"/>
       <c r="D94" s="118" t="s">
         <v>207</v>
       </c>
@@ -9256,10 +9253,10 @@
         <v>130</v>
       </c>
       <c r="F94" s="119"/>
-      <c r="G94" s="335"/>
-      <c r="H94" s="336"/>
-      <c r="I94" s="336"/>
-      <c r="J94" s="337"/>
+      <c r="G94" s="204"/>
+      <c r="H94" s="205"/>
+      <c r="I94" s="205"/>
+      <c r="J94" s="206"/>
       <c r="K94" s="1"/>
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
@@ -9280,11 +9277,11 @@
       <c r="AB94" s="3"/>
     </row>
     <row r="95" spans="1:28" ht="66">
-      <c r="A95" s="331"/>
-      <c r="B95" s="332" t="s">
+      <c r="A95" s="223"/>
+      <c r="B95" s="202" t="s">
         <v>17</v>
       </c>
-      <c r="C95" s="338"/>
+      <c r="C95" s="226"/>
       <c r="D95" s="109" t="s">
         <v>129</v>
       </c>
@@ -9292,10 +9289,10 @@
         <v>206</v>
       </c>
       <c r="F95" s="120"/>
-      <c r="G95" s="336"/>
-      <c r="H95" s="336"/>
-      <c r="I95" s="336"/>
-      <c r="J95" s="339"/>
+      <c r="G95" s="205"/>
+      <c r="H95" s="205"/>
+      <c r="I95" s="205"/>
+      <c r="J95" s="207"/>
       <c r="K95" s="1"/>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
@@ -9316,24 +9313,24 @@
       <c r="AB95" s="3"/>
     </row>
     <row r="96" spans="1:28" ht="49.5">
-      <c r="A96" s="331"/>
-      <c r="B96" s="332" t="s">
+      <c r="A96" s="223"/>
+      <c r="B96" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="C96" s="338"/>
+      <c r="C96" s="226"/>
       <c r="D96" s="188" t="s">
         <v>259</v>
       </c>
       <c r="E96" s="188" t="s">
         <v>258</v>
       </c>
-      <c r="F96" s="356" t="s">
+      <c r="F96" s="218" t="s">
         <v>264</v>
       </c>
-      <c r="G96" s="336"/>
+      <c r="G96" s="205"/>
       <c r="H96" s="23"/>
       <c r="I96" s="23"/>
-      <c r="J96" s="339"/>
+      <c r="J96" s="207"/>
       <c r="K96" s="1"/>
       <c r="L96" s="2"/>
       <c r="M96" s="2"/>
@@ -9354,22 +9351,22 @@
       <c r="AB96" s="3"/>
     </row>
     <row r="97" spans="1:28" ht="49.5">
-      <c r="A97" s="331"/>
-      <c r="B97" s="332" t="s">
+      <c r="A97" s="223"/>
+      <c r="B97" s="202" t="s">
         <v>19</v>
       </c>
-      <c r="C97" s="338"/>
+      <c r="C97" s="226"/>
       <c r="D97" s="109" t="s">
         <v>131</v>
       </c>
       <c r="E97" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="F97" s="334"/>
+      <c r="F97" s="203"/>
       <c r="G97" s="31"/>
       <c r="H97" s="23"/>
-      <c r="I97" s="340"/>
-      <c r="J97" s="339"/>
+      <c r="I97" s="208"/>
+      <c r="J97" s="207"/>
       <c r="K97" s="1"/>
       <c r="L97" s="2"/>
       <c r="M97" s="2"/>
@@ -9390,22 +9387,22 @@
       <c r="AB97" s="3"/>
     </row>
     <row r="98" spans="1:28" ht="66.75" thickBot="1">
-      <c r="A98" s="331"/>
-      <c r="B98" s="332" t="s">
+      <c r="A98" s="223"/>
+      <c r="B98" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="C98" s="338"/>
-      <c r="D98" s="345" t="s">
+      <c r="C98" s="226"/>
+      <c r="D98" s="212" t="s">
         <v>265</v>
       </c>
-      <c r="E98" s="345" t="s">
+      <c r="E98" s="212" t="s">
         <v>266</v>
       </c>
-      <c r="F98" s="357"/>
-      <c r="G98" s="341"/>
+      <c r="F98" s="219"/>
+      <c r="G98" s="209"/>
       <c r="H98" s="189"/>
-      <c r="I98" s="219"/>
-      <c r="J98" s="342"/>
+      <c r="I98" s="227"/>
+      <c r="J98" s="228"/>
       <c r="K98" s="1"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
@@ -9426,16 +9423,16 @@
       <c r="AB98" s="3"/>
     </row>
     <row r="99" spans="1:28" ht="19.5">
-      <c r="A99" s="317"/>
-      <c r="B99" s="318"/>
-      <c r="C99" s="319"/>
-      <c r="D99" s="320"/>
-      <c r="E99" s="321"/>
-      <c r="F99" s="321"/>
-      <c r="G99" s="321"/>
-      <c r="H99" s="321"/>
-      <c r="I99" s="321"/>
-      <c r="J99" s="322"/>
+      <c r="A99" s="191"/>
+      <c r="B99" s="220"/>
+      <c r="C99" s="221"/>
+      <c r="D99" s="192"/>
+      <c r="E99" s="193"/>
+      <c r="F99" s="193"/>
+      <c r="G99" s="193"/>
+      <c r="H99" s="193"/>
+      <c r="I99" s="193"/>
+      <c r="J99" s="194"/>
       <c r="K99" s="1"/>
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
@@ -36457,17 +36454,128 @@
     </row>
   </sheetData>
   <mergeCells count="157">
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="A84:A91"/>
-    <mergeCell ref="C85:C89"/>
-    <mergeCell ref="I89:J89"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="A93:A98"/>
-    <mergeCell ref="C94:C98"/>
-    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="A22:A35"/>
+    <mergeCell ref="C26:C33"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="G1:J2"/>
+    <mergeCell ref="A2:E4"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C10:C20"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="A37:A51"/>
+    <mergeCell ref="A53:A66"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="C41:C49"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="A68:A82"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="C72:C80"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H69:H82"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="I80:J80"/>
+    <mergeCell ref="I81:J81"/>
+    <mergeCell ref="I82:J82"/>
+    <mergeCell ref="D78:E78"/>
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="F70:G70"/>
@@ -36492,128 +36600,17 @@
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A68:A82"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="C72:C80"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H69:H82"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="I78:J78"/>
-    <mergeCell ref="I80:J80"/>
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="I82:J82"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C41:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="A37:A51"/>
-    <mergeCell ref="A53:A66"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="G1:J2"/>
-    <mergeCell ref="A2:E4"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C10:C20"/>
-    <mergeCell ref="A7:A20"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A22:A35"/>
-    <mergeCell ref="C26:C33"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="A84:A91"/>
+    <mergeCell ref="C85:C89"/>
+    <mergeCell ref="I89:J89"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="A93:A98"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="I98:J98"/>
   </mergeCells>
   <pageMargins left="0.216187305364964" right="0.14099172089019399" top="0.26" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="25" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -36624,7 +36621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
@@ -36639,32 +36636,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="313" t="s">
+      <c r="A1" s="353" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="314"/>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
+      <c r="B1" s="354"/>
+      <c r="C1" s="354"/>
+      <c r="D1" s="354"/>
+      <c r="E1" s="354"/>
       <c r="F1" s="175"/>
     </row>
     <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="315" t="s">
+      <c r="A2" s="355" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="315" t="s">
+      <c r="B2" s="355" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="316" t="s">
+      <c r="C2" s="356" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="314"/>
-      <c r="E2" s="314"/>
+      <c r="D2" s="354"/>
+      <c r="E2" s="354"/>
       <c r="F2" s="176"/>
     </row>
     <row r="3" spans="1:6" ht="18">
-      <c r="A3" s="314"/>
-      <c r="B3" s="314"/>
+      <c r="A3" s="354"/>
+      <c r="B3" s="354"/>
       <c r="C3" s="106" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Update: updated for version 1.3
</commit_message>
<xml_diff>
--- a/uploads/xlsx/Timetable SE Department (Fall-25) Version-1.3.xlsx
+++ b/uploads/xlsx/Timetable SE Department (Fall-25) Version-1.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zPythonStuff\Superior Academic Tool\uploads\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096B62A7-202A-479C-BC05-2D6B7E9DB2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4391178B-2248-43D2-8350-8A8858307759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5014,112 +5014,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="118" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5128,172 +5026,124 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5311,6 +5161,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5320,10 +5173,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5347,71 +5200,218 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5645,7 +5645,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
+      <selection pane="bottomLeft" activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5670,10 +5670,10 @@
       <c r="D1" s="128"/>
       <c r="E1" s="128"/>
       <c r="F1" s="128"/>
-      <c r="G1" s="316"/>
-      <c r="H1" s="317"/>
-      <c r="I1" s="317"/>
-      <c r="J1" s="318"/>
+      <c r="G1" s="266"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="268"/>
       <c r="K1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -5694,20 +5694,20 @@
       <c r="AB1" s="3"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A2" s="320" t="s">
+      <c r="A2" s="271" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="321"/>
-      <c r="C2" s="321"/>
-      <c r="D2" s="321"/>
-      <c r="E2" s="321"/>
+      <c r="B2" s="272"/>
+      <c r="C2" s="272"/>
+      <c r="D2" s="272"/>
+      <c r="E2" s="272"/>
       <c r="F2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="310"/>
-      <c r="H2" s="310"/>
-      <c r="I2" s="310"/>
-      <c r="J2" s="319"/>
+      <c r="G2" s="269"/>
+      <c r="H2" s="269"/>
+      <c r="I2" s="269"/>
+      <c r="J2" s="270"/>
       <c r="K2" s="1"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -5728,18 +5728,18 @@
       <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A3" s="322"/>
-      <c r="B3" s="283"/>
-      <c r="C3" s="283"/>
-      <c r="D3" s="283"/>
-      <c r="E3" s="286"/>
+      <c r="A3" s="226"/>
+      <c r="B3" s="273"/>
+      <c r="C3" s="273"/>
+      <c r="D3" s="273"/>
+      <c r="E3" s="274"/>
       <c r="F3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="325"/>
-      <c r="H3" s="301"/>
-      <c r="I3" s="301"/>
-      <c r="J3" s="233"/>
+      <c r="G3" s="276"/>
+      <c r="H3" s="233"/>
+      <c r="I3" s="233"/>
+      <c r="J3" s="237"/>
       <c r="K3" s="4"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -5760,18 +5760,18 @@
       <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:28" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A4" s="323"/>
-      <c r="B4" s="324"/>
-      <c r="C4" s="324"/>
-      <c r="D4" s="324"/>
-      <c r="E4" s="324"/>
+      <c r="A4" s="257"/>
+      <c r="B4" s="275"/>
+      <c r="C4" s="275"/>
+      <c r="D4" s="275"/>
+      <c r="E4" s="275"/>
       <c r="F4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="326"/>
-      <c r="H4" s="327"/>
-      <c r="I4" s="327"/>
-      <c r="J4" s="328"/>
+      <c r="G4" s="277"/>
+      <c r="H4" s="278"/>
+      <c r="I4" s="278"/>
+      <c r="J4" s="279"/>
       <c r="K4" s="4"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -5793,10 +5793,10 @@
     </row>
     <row r="5" spans="1:28" ht="27" customHeight="1" thickBot="1">
       <c r="A5" s="129"/>
-      <c r="B5" s="329" t="s">
+      <c r="B5" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="321"/>
+      <c r="C5" s="272"/>
       <c r="D5" s="146" t="s">
         <v>3</v>
       </c>
@@ -5870,13 +5870,13 @@
       <c r="AB6" s="3"/>
     </row>
     <row r="7" spans="1:28" ht="75" customHeight="1">
-      <c r="A7" s="331" t="s">
+      <c r="A7" s="284" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="263" t="s">
+      <c r="C7" s="288" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="144" t="s">
@@ -5885,17 +5885,17 @@
       <c r="E7" s="144" t="s">
         <v>181</v>
       </c>
-      <c r="F7" s="314" t="s">
+      <c r="F7" s="264" t="s">
         <v>230</v>
       </c>
-      <c r="G7" s="315"/>
+      <c r="G7" s="265"/>
       <c r="H7" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="I7" s="236" t="s">
+      <c r="I7" s="245" t="s">
         <v>215</v>
       </c>
-      <c r="J7" s="233"/>
+      <c r="J7" s="237"/>
       <c r="K7" s="1"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -5916,26 +5916,26 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28" ht="60" customHeight="1">
-      <c r="A8" s="322"/>
+      <c r="A8" s="226"/>
       <c r="B8" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="264"/>
-      <c r="D8" s="313" t="s">
+      <c r="C8" s="282"/>
+      <c r="D8" s="296" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="239"/>
-      <c r="F8" s="249" t="s">
+      <c r="E8" s="246"/>
+      <c r="F8" s="262" t="s">
         <v>220</v>
       </c>
-      <c r="G8" s="336"/>
+      <c r="G8" s="263"/>
       <c r="H8" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="342" t="s">
+      <c r="I8" s="236" t="s">
         <v>193</v>
       </c>
-      <c r="J8" s="233"/>
+      <c r="J8" s="237"/>
       <c r="K8" s="5"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -5956,11 +5956,11 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" ht="61.5" customHeight="1" thickBot="1">
-      <c r="A9" s="322"/>
+      <c r="A9" s="226"/>
       <c r="B9" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="264"/>
+      <c r="C9" s="282"/>
       <c r="D9" s="31" t="s">
         <v>71</v>
       </c>
@@ -5993,11 +5993,11 @@
       <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:28" ht="67.5" customHeight="1">
-      <c r="A10" s="322"/>
+      <c r="A10" s="226"/>
       <c r="B10" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="330" t="s">
+      <c r="C10" s="281" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="31" t="s">
@@ -6006,14 +6006,14 @@
       <c r="E10" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="227" t="s">
+      <c r="F10" s="249" t="s">
         <v>63</v>
       </c>
       <c r="G10" s="240"/>
-      <c r="H10" s="236" t="s">
+      <c r="H10" s="245" t="s">
         <v>90</v>
       </c>
-      <c r="I10" s="239"/>
+      <c r="I10" s="246"/>
       <c r="J10" s="102"/>
       <c r="K10" s="3"/>
       <c r="L10" s="2"/>
@@ -6035,25 +6035,25 @@
       <c r="AB10" s="3"/>
     </row>
     <row r="11" spans="1:28" ht="47.25">
-      <c r="A11" s="322"/>
+      <c r="A11" s="226"/>
       <c r="B11" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="264"/>
-      <c r="D11" s="312" t="s">
+      <c r="C11" s="282"/>
+      <c r="D11" s="294" t="s">
         <v>122</v>
       </c>
-      <c r="E11" s="237"/>
+      <c r="E11" s="287"/>
       <c r="F11" s="23" t="s">
         <v>64</v>
       </c>
       <c r="G11" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="227" t="s">
+      <c r="H11" s="249" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="239"/>
+      <c r="I11" s="246"/>
       <c r="J11" s="103"/>
       <c r="K11" s="5"/>
       <c r="L11" s="2"/>
@@ -6075,22 +6075,22 @@
       <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28" ht="87" customHeight="1">
-      <c r="A12" s="322"/>
+      <c r="A12" s="226"/>
       <c r="B12" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="264"/>
-      <c r="D12" s="279" t="s">
+      <c r="C12" s="282"/>
+      <c r="D12" s="259" t="s">
         <v>231</v>
       </c>
-      <c r="E12" s="239"/>
+      <c r="E12" s="246"/>
       <c r="F12" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="227" t="s">
+      <c r="G12" s="249" t="s">
         <v>262</v>
       </c>
-      <c r="H12" s="239"/>
+      <c r="H12" s="246"/>
       <c r="I12" s="23" t="s">
         <v>68</v>
       </c>
@@ -6115,18 +6115,18 @@
       <c r="AB12" s="3"/>
     </row>
     <row r="13" spans="1:28" ht="47.25">
-      <c r="A13" s="322"/>
+      <c r="A13" s="226"/>
       <c r="B13" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="264"/>
+      <c r="C13" s="282"/>
       <c r="D13" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="335" t="s">
+      <c r="E13" s="261" t="s">
         <v>247</v>
       </c>
-      <c r="F13" s="239"/>
+      <c r="F13" s="246"/>
       <c r="G13" s="23" t="s">
         <v>69</v>
       </c>
@@ -6159,11 +6159,11 @@
       <c r="AB13" s="3"/>
     </row>
     <row r="14" spans="1:28" ht="26.25" hidden="1" customHeight="1">
-      <c r="A14" s="322"/>
+      <c r="A14" s="226"/>
       <c r="B14" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="264"/>
+      <c r="C14" s="282"/>
       <c r="D14" s="48"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
@@ -6191,15 +6191,15 @@
       <c r="AB14" s="3"/>
     </row>
     <row r="15" spans="1:28" ht="63">
-      <c r="A15" s="322"/>
+      <c r="A15" s="226"/>
       <c r="B15" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="264"/>
-      <c r="D15" s="312" t="s">
+      <c r="C15" s="282"/>
+      <c r="D15" s="294" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="237"/>
+      <c r="E15" s="287"/>
       <c r="F15" s="51" t="s">
         <v>147</v>
       </c>
@@ -6209,10 +6209,10 @@
       <c r="H15" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="I15" s="236" t="s">
+      <c r="I15" s="245" t="s">
         <v>141</v>
       </c>
-      <c r="J15" s="233"/>
+      <c r="J15" s="237"/>
       <c r="K15" s="5"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -6233,17 +6233,17 @@
       <c r="AB15" s="3"/>
     </row>
     <row r="16" spans="1:28" ht="57.75" customHeight="1">
-      <c r="A16" s="322"/>
+      <c r="A16" s="226"/>
       <c r="B16" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="264"/>
+      <c r="C16" s="282"/>
       <c r="D16" s="49"/>
       <c r="E16" s="37"/>
-      <c r="F16" s="238" t="s">
+      <c r="F16" s="295" t="s">
         <v>196</v>
       </c>
-      <c r="G16" s="267"/>
+      <c r="G16" s="255"/>
       <c r="H16" s="123"/>
       <c r="I16" s="124"/>
       <c r="J16" s="60"/>
@@ -6267,15 +6267,15 @@
       <c r="AB16" s="3"/>
     </row>
     <row r="17" spans="1:28" ht="71.25" customHeight="1">
-      <c r="A17" s="322"/>
+      <c r="A17" s="226"/>
       <c r="B17" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="264"/>
-      <c r="D17" s="280"/>
-      <c r="E17" s="301"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="242"/>
+      <c r="C17" s="282"/>
+      <c r="D17" s="232"/>
+      <c r="E17" s="233"/>
+      <c r="F17" s="234"/>
+      <c r="G17" s="235"/>
       <c r="H17" s="125"/>
       <c r="I17" s="125"/>
       <c r="J17" s="90"/>
@@ -6299,15 +6299,15 @@
       <c r="AB17" s="3"/>
     </row>
     <row r="18" spans="1:28" ht="64.5" customHeight="1">
-      <c r="A18" s="322"/>
+      <c r="A18" s="226"/>
       <c r="B18" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="264"/>
+      <c r="C18" s="282"/>
       <c r="D18" s="89"/>
       <c r="E18" s="89"/>
-      <c r="F18" s="253"/>
-      <c r="G18" s="242"/>
+      <c r="F18" s="234"/>
+      <c r="G18" s="235"/>
       <c r="H18" s="125"/>
       <c r="I18" s="125"/>
       <c r="J18" s="122"/>
@@ -6331,23 +6331,23 @@
       <c r="AB18" s="3"/>
     </row>
     <row r="19" spans="1:28" ht="60.75" customHeight="1">
-      <c r="A19" s="322"/>
+      <c r="A19" s="226"/>
       <c r="B19" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="264"/>
-      <c r="D19" s="279" t="s">
+      <c r="C19" s="282"/>
+      <c r="D19" s="259" t="s">
         <v>113</v>
       </c>
-      <c r="E19" s="239"/>
-      <c r="F19" s="309" t="s">
+      <c r="E19" s="246"/>
+      <c r="F19" s="290" t="s">
         <v>229</v>
       </c>
-      <c r="G19" s="310"/>
-      <c r="H19" s="241" t="s">
+      <c r="G19" s="269"/>
+      <c r="H19" s="289" t="s">
         <v>137</v>
       </c>
-      <c r="I19" s="242"/>
+      <c r="I19" s="235"/>
       <c r="J19" s="90"/>
       <c r="K19" s="5"/>
       <c r="L19" s="2"/>
@@ -6369,23 +6369,23 @@
       <c r="AB19" s="3"/>
     </row>
     <row r="20" spans="1:28" ht="59.25" customHeight="1" thickBot="1">
-      <c r="A20" s="332"/>
+      <c r="A20" s="285"/>
       <c r="B20" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="265"/>
-      <c r="D20" s="311" t="s">
+      <c r="C20" s="283"/>
+      <c r="D20" s="291" t="s">
         <v>159</v>
       </c>
-      <c r="E20" s="284"/>
-      <c r="F20" s="277" t="s">
+      <c r="E20" s="231"/>
+      <c r="F20" s="230" t="s">
         <v>160</v>
       </c>
-      <c r="G20" s="284"/>
-      <c r="H20" s="293" t="s">
+      <c r="G20" s="231"/>
+      <c r="H20" s="292" t="s">
         <v>161</v>
       </c>
-      <c r="I20" s="294"/>
+      <c r="I20" s="293"/>
       <c r="J20" s="85" t="s">
         <v>191</v>
       </c>
@@ -6410,10 +6410,10 @@
     </row>
     <row r="21" spans="1:28" ht="20.25" thickBot="1">
       <c r="A21" s="41"/>
-      <c r="B21" s="351" t="s">
+      <c r="B21" s="253" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="262"/>
+      <c r="C21" s="254"/>
       <c r="D21" s="27"/>
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
@@ -6441,7 +6441,7 @@
       <c r="AB21" s="3"/>
     </row>
     <row r="22" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A22" s="337" t="s">
+      <c r="A22" s="221" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="91" t="s">
@@ -6489,25 +6489,25 @@
       <c r="AB22" s="3"/>
     </row>
     <row r="23" spans="1:28" ht="47.25" customHeight="1">
-      <c r="A23" s="256"/>
+      <c r="A23" s="222"/>
       <c r="B23" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="352" t="s">
+      <c r="C23" s="256" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="344" t="s">
+      <c r="D23" s="241" t="s">
         <v>212</v>
       </c>
-      <c r="E23" s="345"/>
-      <c r="F23" s="346" t="s">
+      <c r="E23" s="242"/>
+      <c r="F23" s="243" t="s">
         <v>138</v>
       </c>
-      <c r="G23" s="345"/>
-      <c r="H23" s="347" t="s">
+      <c r="G23" s="242"/>
+      <c r="H23" s="244" t="s">
         <v>177</v>
       </c>
-      <c r="I23" s="345"/>
+      <c r="I23" s="242"/>
       <c r="J23" s="99" t="s">
         <v>12</v>
       </c>
@@ -6531,23 +6531,23 @@
       <c r="AB23" s="3"/>
     </row>
     <row r="24" spans="1:28" ht="52.5" customHeight="1">
-      <c r="A24" s="256"/>
+      <c r="A24" s="222"/>
       <c r="B24" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="322"/>
-      <c r="D24" s="236" t="s">
+      <c r="C24" s="226"/>
+      <c r="D24" s="245" t="s">
         <v>208</v>
       </c>
-      <c r="E24" s="239"/>
-      <c r="F24" s="236" t="s">
+      <c r="E24" s="246"/>
+      <c r="F24" s="245" t="s">
         <v>175</v>
       </c>
-      <c r="G24" s="239"/>
-      <c r="H24" s="236" t="s">
+      <c r="G24" s="246"/>
+      <c r="H24" s="245" t="s">
         <v>116</v>
       </c>
-      <c r="I24" s="239"/>
+      <c r="I24" s="246"/>
       <c r="J24" s="59" t="s">
         <v>12</v>
       </c>
@@ -6571,11 +6571,11 @@
       <c r="AB24" s="3"/>
     </row>
     <row r="25" spans="1:28" ht="81" customHeight="1" thickBot="1">
-      <c r="A25" s="256"/>
+      <c r="A25" s="222"/>
       <c r="B25" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="323"/>
+      <c r="C25" s="257"/>
       <c r="D25" s="51"/>
       <c r="E25" s="51" t="s">
         <v>219</v>
@@ -6583,14 +6583,14 @@
       <c r="F25" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="227" t="s">
+      <c r="G25" s="249" t="s">
         <v>246</v>
       </c>
-      <c r="H25" s="349"/>
-      <c r="I25" s="350" t="s">
+      <c r="H25" s="250"/>
+      <c r="I25" s="251" t="s">
         <v>248</v>
       </c>
-      <c r="J25" s="245"/>
+      <c r="J25" s="252"/>
       <c r="K25" s="7"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -6611,27 +6611,27 @@
       <c r="AB25" s="3"/>
     </row>
     <row r="26" spans="1:28" ht="47.25">
-      <c r="A26" s="256"/>
+      <c r="A26" s="222"/>
       <c r="B26" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="338" t="s">
+      <c r="C26" s="224" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="333" t="s">
+      <c r="D26" s="258" t="s">
         <v>194</v>
       </c>
-      <c r="E26" s="239"/>
+      <c r="E26" s="246"/>
       <c r="F26" s="69" t="s">
         <v>64</v>
       </c>
       <c r="G26" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="227" t="s">
+      <c r="H26" s="249" t="s">
         <v>73</v>
       </c>
-      <c r="I26" s="239"/>
+      <c r="I26" s="246"/>
       <c r="J26" s="61"/>
       <c r="K26" s="6"/>
       <c r="L26" s="2"/>
@@ -6653,11 +6653,11 @@
       <c r="AB26" s="3"/>
     </row>
     <row r="27" spans="1:28" ht="47.25">
-      <c r="A27" s="256"/>
+      <c r="A27" s="222"/>
       <c r="B27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="296"/>
+      <c r="C27" s="225"/>
       <c r="D27" s="51" t="s">
         <v>184</v>
       </c>
@@ -6670,10 +6670,10 @@
       <c r="G27" s="151" t="s">
         <v>172</v>
       </c>
-      <c r="H27" s="279" t="s">
+      <c r="H27" s="259" t="s">
         <v>143</v>
       </c>
-      <c r="I27" s="239"/>
+      <c r="I27" s="246"/>
       <c r="J27" s="64" t="s">
         <v>190</v>
       </c>
@@ -6697,25 +6697,25 @@
       <c r="AB27" s="3"/>
     </row>
     <row r="28" spans="1:28" ht="63">
-      <c r="A28" s="256"/>
+      <c r="A28" s="222"/>
       <c r="B28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="296"/>
+      <c r="C28" s="225"/>
       <c r="D28" s="105" t="s">
         <v>221</v>
       </c>
       <c r="E28" s="70" t="s">
         <v>187</v>
       </c>
-      <c r="F28" s="302" t="s">
+      <c r="F28" s="238" t="s">
         <v>213</v>
       </c>
-      <c r="G28" s="343"/>
-      <c r="H28" s="227" t="s">
+      <c r="G28" s="239"/>
+      <c r="H28" s="249" t="s">
         <v>74</v>
       </c>
-      <c r="I28" s="239"/>
+      <c r="I28" s="246"/>
       <c r="J28" s="90"/>
       <c r="K28" s="6"/>
       <c r="L28" s="2"/>
@@ -6737,11 +6737,11 @@
       <c r="AB28" s="3"/>
     </row>
     <row r="29" spans="1:28" ht="62.25" customHeight="1">
-      <c r="A29" s="256"/>
+      <c r="A29" s="222"/>
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="296"/>
+      <c r="C29" s="225"/>
       <c r="D29" s="23" t="s">
         <v>61</v>
       </c>
@@ -6783,26 +6783,26 @@
       <c r="AB29" s="3"/>
     </row>
     <row r="30" spans="1:28" ht="63">
-      <c r="A30" s="256"/>
+      <c r="A30" s="222"/>
       <c r="B30" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="296"/>
-      <c r="D30" s="348" t="s">
+      <c r="C30" s="225"/>
+      <c r="D30" s="247" t="s">
         <v>234</v>
       </c>
-      <c r="E30" s="252"/>
-      <c r="F30" s="334" t="s">
+      <c r="E30" s="248"/>
+      <c r="F30" s="260" t="s">
         <v>188</v>
       </c>
-      <c r="G30" s="239"/>
+      <c r="G30" s="246"/>
       <c r="H30" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="I30" s="227" t="s">
+      <c r="I30" s="249" t="s">
         <v>244</v>
       </c>
-      <c r="J30" s="233"/>
+      <c r="J30" s="237"/>
       <c r="K30" s="6"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -6823,19 +6823,19 @@
       <c r="AB30" s="3"/>
     </row>
     <row r="31" spans="1:28" ht="60.75" customHeight="1">
-      <c r="A31" s="256"/>
+      <c r="A31" s="222"/>
       <c r="B31" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="296"/>
+      <c r="C31" s="225"/>
       <c r="D31" s="134"/>
       <c r="E31" s="135"/>
       <c r="F31" s="136"/>
       <c r="G31" s="137"/>
-      <c r="H31" s="348" t="s">
+      <c r="H31" s="247" t="s">
         <v>226</v>
       </c>
-      <c r="I31" s="267"/>
+      <c r="I31" s="255"/>
       <c r="J31" s="61"/>
       <c r="K31" s="6"/>
       <c r="L31" s="2"/>
@@ -6857,11 +6857,11 @@
       <c r="AB31" s="3"/>
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
-      <c r="A32" s="256"/>
+      <c r="A32" s="222"/>
       <c r="B32" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="322"/>
+      <c r="C32" s="226"/>
       <c r="D32" s="125"/>
       <c r="E32" s="125"/>
       <c r="F32" s="125"/>
@@ -6889,11 +6889,11 @@
       <c r="AB32" s="3"/>
     </row>
     <row r="33" spans="1:28" ht="54.75" customHeight="1">
-      <c r="A33" s="256"/>
+      <c r="A33" s="222"/>
       <c r="B33" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="339"/>
+      <c r="C33" s="227"/>
       <c r="D33" s="125"/>
       <c r="E33" s="125"/>
       <c r="F33" s="125"/>
@@ -6921,22 +6921,22 @@
       <c r="AB33" s="3"/>
     </row>
     <row r="34" spans="1:28" ht="49.5">
-      <c r="A34" s="256"/>
+      <c r="A34" s="222"/>
       <c r="B34" s="18" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="302" t="s">
+      <c r="D34" s="238" t="s">
         <v>201</v>
       </c>
       <c r="E34" s="240"/>
-      <c r="F34" s="302" t="s">
+      <c r="F34" s="238" t="s">
         <v>111</v>
       </c>
       <c r="G34" s="240"/>
-      <c r="H34" s="302" t="s">
+      <c r="H34" s="238" t="s">
         <v>222</v>
       </c>
       <c r="I34" s="240"/>
@@ -6961,19 +6961,19 @@
       <c r="AB34" s="3"/>
     </row>
     <row r="35" spans="1:28" ht="53.25" thickBot="1">
-      <c r="A35" s="257"/>
+      <c r="A35" s="223"/>
       <c r="B35" s="78" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="141" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="340" t="s">
+      <c r="D35" s="228" t="s">
         <v>251</v>
       </c>
-      <c r="E35" s="341"/>
-      <c r="F35" s="277"/>
-      <c r="G35" s="284"/>
+      <c r="E35" s="229"/>
+      <c r="F35" s="230"/>
+      <c r="G35" s="231"/>
       <c r="H35" s="84" t="s">
         <v>233</v>
       </c>
@@ -7000,10 +7000,10 @@
     </row>
     <row r="36" spans="1:28" ht="20.25" thickBot="1">
       <c r="A36" s="45"/>
-      <c r="B36" s="285" t="s">
+      <c r="B36" s="310" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="286"/>
+      <c r="C36" s="274"/>
       <c r="D36" s="27"/>
       <c r="E36" s="42"/>
       <c r="F36" s="42"/>
@@ -7031,7 +7031,7 @@
       <c r="AB36" s="3"/>
     </row>
     <row r="37" spans="1:28" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A37" s="295" t="s">
+      <c r="A37" s="298" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="53" t="s">
@@ -7079,11 +7079,11 @@
       <c r="AB37" s="3"/>
     </row>
     <row r="38" spans="1:28" ht="52.5" customHeight="1">
-      <c r="A38" s="296"/>
+      <c r="A38" s="225"/>
       <c r="B38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="287" t="s">
+      <c r="C38" s="311" t="s">
         <v>30</v>
       </c>
       <c r="D38" s="22" t="s">
@@ -7092,14 +7092,14 @@
       <c r="E38" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="227" t="s">
+      <c r="F38" s="249" t="s">
         <v>140</v>
       </c>
-      <c r="G38" s="239"/>
-      <c r="H38" s="236" t="s">
+      <c r="G38" s="246"/>
+      <c r="H38" s="245" t="s">
         <v>173</v>
       </c>
-      <c r="I38" s="239"/>
+      <c r="I38" s="246"/>
       <c r="J38" s="59" t="s">
         <v>12</v>
       </c>
@@ -7123,23 +7123,23 @@
       <c r="AB38" s="3"/>
     </row>
     <row r="39" spans="1:28" ht="58.5" customHeight="1">
-      <c r="A39" s="296"/>
+      <c r="A39" s="225"/>
       <c r="B39" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="269"/>
-      <c r="D39" s="236" t="s">
+      <c r="C39" s="312"/>
+      <c r="D39" s="245" t="s">
         <v>174</v>
       </c>
       <c r="E39" s="240"/>
-      <c r="F39" s="238" t="s">
+      <c r="F39" s="295" t="s">
         <v>216</v>
       </c>
-      <c r="G39" s="239"/>
-      <c r="H39" s="227" t="s">
+      <c r="G39" s="246"/>
+      <c r="H39" s="249" t="s">
         <v>139</v>
       </c>
-      <c r="I39" s="239"/>
+      <c r="I39" s="246"/>
       <c r="J39" s="59" t="s">
         <v>12</v>
       </c>
@@ -7163,15 +7163,15 @@
       <c r="AB39" s="3"/>
     </row>
     <row r="40" spans="1:28" ht="57" customHeight="1">
-      <c r="A40" s="296"/>
+      <c r="A40" s="225"/>
       <c r="B40" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="288"/>
-      <c r="D40" s="236" t="s">
+      <c r="C40" s="313"/>
+      <c r="D40" s="245" t="s">
         <v>123</v>
       </c>
-      <c r="E40" s="301"/>
+      <c r="E40" s="233"/>
       <c r="F40" s="125"/>
       <c r="G40" s="89"/>
       <c r="H40" s="22" t="s">
@@ -7203,26 +7203,26 @@
       <c r="AB40" s="3"/>
     </row>
     <row r="41" spans="1:28" ht="55.5" customHeight="1">
-      <c r="A41" s="296"/>
+      <c r="A41" s="225"/>
       <c r="B41" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="289" t="s">
+      <c r="C41" s="314" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="236" t="s">
+      <c r="D41" s="245" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="237"/>
-      <c r="F41" s="251" t="s">
+      <c r="E41" s="287"/>
+      <c r="F41" s="342" t="s">
         <v>76</v>
       </c>
-      <c r="G41" s="252"/>
+      <c r="G41" s="248"/>
       <c r="H41" s="23"/>
-      <c r="I41" s="227" t="s">
+      <c r="I41" s="249" t="s">
         <v>91</v>
       </c>
-      <c r="J41" s="245"/>
+      <c r="J41" s="252"/>
       <c r="K41" s="6"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
@@ -7243,15 +7243,15 @@
       <c r="AB41" s="3"/>
     </row>
     <row r="42" spans="1:28" ht="64.5" customHeight="1">
-      <c r="A42" s="296"/>
+      <c r="A42" s="225"/>
       <c r="B42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="269"/>
-      <c r="D42" s="236" t="s">
+      <c r="C42" s="312"/>
+      <c r="D42" s="245" t="s">
         <v>168</v>
       </c>
-      <c r="E42" s="301"/>
+      <c r="E42" s="233"/>
       <c r="F42" s="154" t="s">
         <v>78</v>
       </c>
@@ -7287,22 +7287,22 @@
       <c r="AB42" s="3"/>
     </row>
     <row r="43" spans="1:28" ht="108.75" customHeight="1">
-      <c r="A43" s="296"/>
+      <c r="A43" s="225"/>
       <c r="B43" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="269"/>
-      <c r="D43" s="227" t="s">
+      <c r="C43" s="312"/>
+      <c r="D43" s="249" t="s">
         <v>232</v>
       </c>
-      <c r="E43" s="237"/>
+      <c r="E43" s="287"/>
       <c r="F43" s="144" t="s">
         <v>214</v>
       </c>
-      <c r="G43" s="302" t="s">
+      <c r="G43" s="238" t="s">
         <v>260</v>
       </c>
-      <c r="H43" s="239"/>
+      <c r="H43" s="246"/>
       <c r="I43" s="89"/>
       <c r="J43" s="90"/>
       <c r="K43" s="6"/>
@@ -7325,22 +7325,22 @@
       <c r="AB43" s="3"/>
     </row>
     <row r="44" spans="1:28" ht="63" customHeight="1">
-      <c r="A44" s="296"/>
+      <c r="A44" s="225"/>
       <c r="B44" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="269"/>
-      <c r="D44" s="236" t="s">
+      <c r="C44" s="312"/>
+      <c r="D44" s="245" t="s">
         <v>186</v>
       </c>
-      <c r="E44" s="237"/>
+      <c r="E44" s="287"/>
       <c r="F44" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="G44" s="236" t="s">
+      <c r="G44" s="245" t="s">
         <v>93</v>
       </c>
-      <c r="H44" s="239"/>
+      <c r="H44" s="246"/>
       <c r="I44" s="26"/>
       <c r="J44" s="61"/>
       <c r="K44" s="6"/>
@@ -7363,13 +7363,13 @@
       <c r="AB44" s="3"/>
     </row>
     <row r="45" spans="1:28" ht="64.5" hidden="1" customHeight="1">
-      <c r="A45" s="296"/>
+      <c r="A45" s="225"/>
       <c r="B45" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="269"/>
+      <c r="C45" s="312"/>
       <c r="D45" s="303"/>
-      <c r="E45" s="239"/>
+      <c r="E45" s="246"/>
       <c r="F45" s="26"/>
       <c r="G45" s="39"/>
       <c r="H45" s="26"/>
@@ -7395,11 +7395,11 @@
       <c r="AB45" s="3"/>
     </row>
     <row r="46" spans="1:28" ht="47.25">
-      <c r="A46" s="296"/>
+      <c r="A46" s="225"/>
       <c r="B46" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="269"/>
+      <c r="C46" s="312"/>
       <c r="D46" s="66" t="s">
         <v>79</v>
       </c>
@@ -7412,10 +7412,10 @@
       <c r="G46" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="H46" s="236" t="s">
+      <c r="H46" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="I46" s="239"/>
+      <c r="I46" s="246"/>
       <c r="J46" s="64" t="s">
         <v>32</v>
       </c>
@@ -7439,19 +7439,19 @@
       <c r="AB46" s="3"/>
     </row>
     <row r="47" spans="1:28" ht="50.25" customHeight="1">
-      <c r="A47" s="296"/>
+      <c r="A47" s="225"/>
       <c r="B47" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="269"/>
+      <c r="C47" s="312"/>
       <c r="D47" s="134"/>
       <c r="E47" s="135"/>
       <c r="F47" s="136"/>
       <c r="G47" s="137"/>
-      <c r="H47" s="238" t="s">
+      <c r="H47" s="295" t="s">
         <v>167</v>
       </c>
-      <c r="I47" s="267"/>
+      <c r="I47" s="255"/>
       <c r="J47" s="60"/>
       <c r="K47" s="6"/>
       <c r="L47" s="2"/>
@@ -7473,11 +7473,11 @@
       <c r="AB47" s="3"/>
     </row>
     <row r="48" spans="1:28" ht="49.5" customHeight="1">
-      <c r="A48" s="296"/>
+      <c r="A48" s="225"/>
       <c r="B48" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="290"/>
+      <c r="C48" s="315"/>
       <c r="D48" s="125"/>
       <c r="E48" s="125"/>
       <c r="F48" s="125"/>
@@ -7505,15 +7505,15 @@
       <c r="AB48" s="3"/>
     </row>
     <row r="49" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A49" s="296"/>
+      <c r="A49" s="225"/>
       <c r="B49" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C49" s="291"/>
-      <c r="D49" s="253" t="s">
+      <c r="C49" s="316"/>
+      <c r="D49" s="234" t="s">
         <v>115</v>
       </c>
-      <c r="E49" s="242"/>
+      <c r="E49" s="235"/>
       <c r="F49" s="125"/>
       <c r="G49" s="125"/>
       <c r="H49" s="125"/>
@@ -7539,7 +7539,7 @@
       <c r="AB49" s="3"/>
     </row>
     <row r="50" spans="1:28" ht="49.5">
-      <c r="A50" s="296"/>
+      <c r="A50" s="225"/>
       <c r="B50" s="19" t="s">
         <v>25</v>
       </c>
@@ -7550,14 +7550,14 @@
         <v>181</v>
       </c>
       <c r="E50" s="145"/>
-      <c r="F50" s="241" t="s">
+      <c r="F50" s="289" t="s">
         <v>236</v>
       </c>
-      <c r="G50" s="242"/>
-      <c r="H50" s="241" t="s">
+      <c r="G50" s="235"/>
+      <c r="H50" s="289" t="s">
         <v>210</v>
       </c>
-      <c r="I50" s="242"/>
+      <c r="I50" s="235"/>
       <c r="J50" s="122"/>
       <c r="K50" s="8"/>
       <c r="L50" s="2"/>
@@ -7579,7 +7579,7 @@
       <c r="AB50" s="3"/>
     </row>
     <row r="51" spans="1:28" ht="79.5" thickBot="1">
-      <c r="A51" s="297"/>
+      <c r="A51" s="299"/>
       <c r="B51" s="62" t="s">
         <v>26</v>
       </c>
@@ -7592,14 +7592,14 @@
       <c r="E51" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="F51" s="246" t="s">
+      <c r="F51" s="338" t="s">
         <v>238</v>
       </c>
-      <c r="G51" s="247"/>
-      <c r="H51" s="293" t="s">
+      <c r="G51" s="339"/>
+      <c r="H51" s="292" t="s">
         <v>162</v>
       </c>
-      <c r="I51" s="294"/>
+      <c r="I51" s="293"/>
       <c r="J51" s="85" t="s">
         <v>163</v>
       </c>
@@ -7624,10 +7624,10 @@
     </row>
     <row r="52" spans="1:28" ht="21.75" customHeight="1" thickBot="1">
       <c r="A52" s="46"/>
-      <c r="B52" s="292" t="s">
+      <c r="B52" s="317" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="262"/>
+      <c r="C52" s="254"/>
       <c r="D52" s="27"/>
       <c r="E52" s="28"/>
       <c r="F52" s="28"/>
@@ -7655,7 +7655,7 @@
       <c r="AB52" s="3"/>
     </row>
     <row r="53" spans="1:28" ht="19.5">
-      <c r="A53" s="298" t="s">
+      <c r="A53" s="300" t="s">
         <v>33</v>
       </c>
       <c r="B53" s="160" t="s">
@@ -7703,25 +7703,25 @@
       <c r="AB53" s="3"/>
     </row>
     <row r="54" spans="1:28" ht="56.25" customHeight="1">
-      <c r="A54" s="299"/>
+      <c r="A54" s="301"/>
       <c r="B54" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="258" t="s">
+      <c r="C54" s="320" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="253" t="s">
+      <c r="D54" s="234" t="s">
         <v>178</v>
       </c>
-      <c r="E54" s="242"/>
-      <c r="F54" s="253" t="s">
+      <c r="E54" s="235"/>
+      <c r="F54" s="234" t="s">
         <v>176</v>
       </c>
-      <c r="G54" s="242"/>
-      <c r="H54" s="253" t="s">
+      <c r="G54" s="235"/>
+      <c r="H54" s="234" t="s">
         <v>218</v>
       </c>
-      <c r="I54" s="242"/>
+      <c r="I54" s="235"/>
       <c r="J54" s="164" t="s">
         <v>12</v>
       </c>
@@ -7745,24 +7745,24 @@
       <c r="AB54" s="3"/>
     </row>
     <row r="55" spans="1:28" ht="60" customHeight="1">
-      <c r="A55" s="299"/>
+      <c r="A55" s="301"/>
       <c r="B55" s="155" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="242"/>
-      <c r="D55" s="253" t="s">
+      <c r="C55" s="235"/>
+      <c r="D55" s="234" t="s">
         <v>154</v>
       </c>
-      <c r="E55" s="242"/>
-      <c r="F55" s="253" t="s">
+      <c r="E55" s="235"/>
+      <c r="F55" s="234" t="s">
         <v>155</v>
       </c>
-      <c r="G55" s="242"/>
+      <c r="G55" s="235"/>
       <c r="H55" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="I55" s="234"/>
-      <c r="J55" s="235"/>
+      <c r="I55" s="334"/>
+      <c r="J55" s="335"/>
       <c r="K55" s="5"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
@@ -7783,28 +7783,28 @@
       <c r="AB55" s="3"/>
     </row>
     <row r="56" spans="1:28" ht="78" customHeight="1">
-      <c r="A56" s="299"/>
+      <c r="A56" s="301"/>
       <c r="B56" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="242"/>
+      <c r="C56" s="235"/>
       <c r="D56" s="156" t="s">
         <v>12</v>
       </c>
       <c r="E56" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="F56" s="241" t="s">
+      <c r="F56" s="289" t="s">
         <v>142</v>
       </c>
-      <c r="G56" s="242"/>
+      <c r="G56" s="235"/>
       <c r="H56" s="151" t="s">
         <v>83</v>
       </c>
-      <c r="I56" s="253" t="s">
+      <c r="I56" s="234" t="s">
         <v>164</v>
       </c>
-      <c r="J56" s="254"/>
+      <c r="J56" s="297"/>
       <c r="K56" s="6"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
@@ -7825,21 +7825,21 @@
       <c r="AB56" s="3"/>
     </row>
     <row r="57" spans="1:28" ht="47.25">
-      <c r="A57" s="299"/>
+      <c r="A57" s="301"/>
       <c r="B57" s="155" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="259" t="s">
+      <c r="C57" s="321" t="s">
         <v>16</v>
       </c>
-      <c r="D57" s="243" t="s">
+      <c r="D57" s="336" t="s">
         <v>249</v>
       </c>
-      <c r="E57" s="244"/>
-      <c r="F57" s="248" t="s">
+      <c r="E57" s="337"/>
+      <c r="F57" s="340" t="s">
         <v>240</v>
       </c>
-      <c r="G57" s="248"/>
+      <c r="G57" s="340"/>
       <c r="H57" s="151" t="s">
         <v>81</v>
       </c>
@@ -7867,11 +7867,11 @@
       <c r="AB57" s="3"/>
     </row>
     <row r="58" spans="1:28" ht="60" customHeight="1">
-      <c r="A58" s="299"/>
+      <c r="A58" s="301"/>
       <c r="B58" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="242"/>
+      <c r="C58" s="235"/>
       <c r="D58" s="157" t="s">
         <v>149</v>
       </c>
@@ -7884,10 +7884,10 @@
       <c r="G58" s="151" t="s">
         <v>237</v>
       </c>
-      <c r="H58" s="241" t="s">
+      <c r="H58" s="289" t="s">
         <v>77</v>
       </c>
-      <c r="I58" s="241"/>
+      <c r="I58" s="289"/>
       <c r="J58" s="166"/>
       <c r="K58" s="5"/>
       <c r="L58" s="2"/>
@@ -7909,15 +7909,15 @@
       <c r="AB58" s="3"/>
     </row>
     <row r="59" spans="1:28" ht="54" customHeight="1">
-      <c r="A59" s="299"/>
+      <c r="A59" s="301"/>
       <c r="B59" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="242"/>
-      <c r="D59" s="253" t="s">
+      <c r="C59" s="235"/>
+      <c r="D59" s="234" t="s">
         <v>84</v>
       </c>
-      <c r="E59" s="242"/>
+      <c r="E59" s="235"/>
       <c r="F59" s="151" t="s">
         <v>225</v>
       </c>
@@ -7951,15 +7951,15 @@
       <c r="AB59" s="3"/>
     </row>
     <row r="60" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A60" s="299"/>
+      <c r="A60" s="301"/>
       <c r="B60" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="242"/>
-      <c r="D60" s="253" t="s">
+      <c r="C60" s="235"/>
+      <c r="D60" s="234" t="s">
         <v>95</v>
       </c>
-      <c r="E60" s="242"/>
+      <c r="E60" s="235"/>
       <c r="F60" s="150" t="s">
         <v>97</v>
       </c>
@@ -7993,11 +7993,11 @@
       <c r="AB60" s="3"/>
     </row>
     <row r="61" spans="1:28" ht="47.25">
-      <c r="A61" s="299"/>
+      <c r="A61" s="301"/>
       <c r="B61" s="155" t="s">
         <v>21</v>
       </c>
-      <c r="C61" s="242"/>
+      <c r="C61" s="235"/>
       <c r="D61" s="125"/>
       <c r="E61" s="125"/>
       <c r="F61" s="157" t="s">
@@ -8009,10 +8009,10 @@
       <c r="H61" s="150" t="s">
         <v>183</v>
       </c>
-      <c r="I61" s="241" t="s">
+      <c r="I61" s="289" t="s">
         <v>245</v>
       </c>
-      <c r="J61" s="254"/>
+      <c r="J61" s="297"/>
       <c r="K61" s="5"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
@@ -8033,17 +8033,17 @@
       <c r="AB61" s="3"/>
     </row>
     <row r="62" spans="1:28" ht="47.25" customHeight="1">
-      <c r="A62" s="299"/>
+      <c r="A62" s="301"/>
       <c r="B62" s="155" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="242"/>
+      <c r="C62" s="235"/>
       <c r="D62" s="158"/>
       <c r="E62" s="158"/>
-      <c r="F62" s="253" t="s">
+      <c r="F62" s="234" t="s">
         <v>165</v>
       </c>
-      <c r="G62" s="242"/>
+      <c r="G62" s="235"/>
       <c r="H62" s="304" t="s">
         <v>169</v>
       </c>
@@ -8069,11 +8069,11 @@
       <c r="AB62" s="3"/>
     </row>
     <row r="63" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A63" s="299"/>
+      <c r="A63" s="301"/>
       <c r="B63" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="260" t="s">
+      <c r="C63" s="322" t="s">
         <v>16</v>
       </c>
       <c r="D63" s="125"/>
@@ -8103,19 +8103,19 @@
       <c r="AB63" s="3"/>
     </row>
     <row r="64" spans="1:28" ht="51" customHeight="1">
-      <c r="A64" s="299"/>
+      <c r="A64" s="301"/>
       <c r="B64" s="155" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="242"/>
+      <c r="C64" s="235"/>
       <c r="D64" s="125"/>
       <c r="E64" s="125"/>
       <c r="F64" s="125"/>
       <c r="G64" s="125"/>
-      <c r="H64" s="253" t="s">
+      <c r="H64" s="234" t="s">
         <v>179</v>
       </c>
-      <c r="I64" s="242"/>
+      <c r="I64" s="235"/>
       <c r="J64" s="167"/>
       <c r="K64" s="5"/>
       <c r="L64" s="2"/>
@@ -8137,7 +8137,7 @@
       <c r="AB64" s="3"/>
     </row>
     <row r="65" spans="1:28" ht="50.25" customHeight="1">
-      <c r="A65" s="299"/>
+      <c r="A65" s="301"/>
       <c r="B65" s="155" t="s">
         <v>25</v>
       </c>
@@ -8150,14 +8150,14 @@
       <c r="E65" s="150" t="s">
         <v>158</v>
       </c>
-      <c r="F65" s="253" t="s">
+      <c r="F65" s="234" t="s">
         <v>170</v>
       </c>
-      <c r="G65" s="242"/>
-      <c r="H65" s="253" t="s">
+      <c r="G65" s="235"/>
+      <c r="H65" s="234" t="s">
         <v>217</v>
       </c>
-      <c r="I65" s="242"/>
+      <c r="I65" s="235"/>
       <c r="J65" s="166"/>
       <c r="K65" s="5"/>
       <c r="L65" s="2"/>
@@ -8179,7 +8179,7 @@
       <c r="AB65" s="3"/>
     </row>
     <row r="66" spans="1:28" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A66" s="300"/>
+      <c r="A66" s="302"/>
       <c r="B66" s="168" t="s">
         <v>26</v>
       </c>
@@ -8222,10 +8222,10 @@
     </row>
     <row r="67" spans="1:28" ht="20.25" thickBot="1">
       <c r="A67" s="46"/>
-      <c r="B67" s="261" t="s">
+      <c r="B67" s="323" t="s">
         <v>35</v>
       </c>
-      <c r="C67" s="262"/>
+      <c r="C67" s="254"/>
       <c r="D67" s="27"/>
       <c r="E67" s="32"/>
       <c r="F67" s="32"/>
@@ -8253,7 +8253,7 @@
       <c r="AB67" s="3"/>
     </row>
     <row r="68" spans="1:28" ht="61.5" customHeight="1" thickBot="1">
-      <c r="A68" s="255" t="s">
+      <c r="A68" s="319" t="s">
         <v>36</v>
       </c>
       <c r="B68" s="71" t="s">
@@ -8299,11 +8299,11 @@
       <c r="AB68" s="3"/>
     </row>
     <row r="69" spans="1:28" ht="64.5" customHeight="1">
-      <c r="A69" s="256"/>
+      <c r="A69" s="222"/>
       <c r="B69" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="263" t="s">
+      <c r="C69" s="288" t="s">
         <v>43</v>
       </c>
       <c r="D69" s="47" t="s">
@@ -8318,7 +8318,7 @@
       <c r="G69" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="268" t="s">
+      <c r="H69" s="325" t="s">
         <v>185</v>
       </c>
       <c r="I69" s="22" t="s">
@@ -8347,26 +8347,26 @@
       <c r="AB69" s="3"/>
     </row>
     <row r="70" spans="1:28" ht="50.25" customHeight="1">
-      <c r="A70" s="256"/>
+      <c r="A70" s="222"/>
       <c r="B70" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="264"/>
+      <c r="C70" s="282"/>
       <c r="D70" s="47" t="s">
         <v>12</v>
       </c>
       <c r="E70" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="236" t="s">
+      <c r="F70" s="245" t="s">
         <v>96</v>
       </c>
-      <c r="G70" s="237"/>
-      <c r="H70" s="269"/>
-      <c r="I70" s="249" t="s">
+      <c r="G70" s="287"/>
+      <c r="H70" s="312"/>
+      <c r="I70" s="262" t="s">
         <v>241</v>
       </c>
-      <c r="J70" s="250"/>
+      <c r="J70" s="341"/>
       <c r="K70" s="6"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
@@ -8387,24 +8387,24 @@
       <c r="AB70" s="3"/>
     </row>
     <row r="71" spans="1:28" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A71" s="256"/>
+      <c r="A71" s="222"/>
       <c r="B71" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C71" s="265"/>
-      <c r="D71" s="271" t="s">
+      <c r="C71" s="283"/>
+      <c r="D71" s="327" t="s">
         <v>202</v>
       </c>
-      <c r="E71" s="272"/>
+      <c r="E71" s="328"/>
       <c r="F71" s="121"/>
       <c r="G71" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="H71" s="269"/>
-      <c r="I71" s="232" t="s">
+      <c r="H71" s="312"/>
+      <c r="I71" s="318" t="s">
         <v>203</v>
       </c>
-      <c r="J71" s="233"/>
+      <c r="J71" s="237"/>
       <c r="K71" s="6"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
@@ -8425,26 +8425,26 @@
       <c r="AB71" s="3"/>
     </row>
     <row r="72" spans="1:28" ht="52.5" customHeight="1">
-      <c r="A72" s="256"/>
+      <c r="A72" s="222"/>
       <c r="B72" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C72" s="266" t="s">
+      <c r="C72" s="324" t="s">
         <v>16</v>
       </c>
-      <c r="D72" s="271" t="s">
+      <c r="D72" s="327" t="s">
         <v>86</v>
       </c>
-      <c r="E72" s="272"/>
-      <c r="F72" s="236" t="s">
+      <c r="E72" s="328"/>
+      <c r="F72" s="245" t="s">
         <v>192</v>
       </c>
-      <c r="G72" s="233"/>
-      <c r="H72" s="269"/>
-      <c r="I72" s="232" t="s">
+      <c r="G72" s="237"/>
+      <c r="H72" s="312"/>
+      <c r="I72" s="318" t="s">
         <v>87</v>
       </c>
-      <c r="J72" s="233"/>
+      <c r="J72" s="237"/>
       <c r="K72" s="6"/>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
@@ -8465,26 +8465,26 @@
       <c r="AB72" s="3"/>
     </row>
     <row r="73" spans="1:28" ht="61.5" customHeight="1">
-      <c r="A73" s="256"/>
+      <c r="A73" s="222"/>
       <c r="B73" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C73" s="264"/>
+      <c r="C73" s="282"/>
       <c r="D73" s="88" t="s">
         <v>153</v>
       </c>
       <c r="E73" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="F73" s="273" t="s">
+      <c r="F73" s="329" t="s">
         <v>253</v>
       </c>
-      <c r="G73" s="274"/>
-      <c r="H73" s="269"/>
-      <c r="I73" s="273" t="s">
+      <c r="G73" s="330"/>
+      <c r="H73" s="312"/>
+      <c r="I73" s="329" t="s">
         <v>254</v>
       </c>
-      <c r="J73" s="275"/>
+      <c r="J73" s="331"/>
       <c r="K73" s="6"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
@@ -8505,24 +8505,24 @@
       <c r="AB73" s="3"/>
     </row>
     <row r="74" spans="1:28" ht="60.75" customHeight="1">
-      <c r="A74" s="256"/>
+      <c r="A74" s="222"/>
       <c r="B74" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C74" s="264"/>
-      <c r="D74" s="279" t="s">
+      <c r="C74" s="282"/>
+      <c r="D74" s="259" t="s">
         <v>180</v>
       </c>
-      <c r="E74" s="239"/>
-      <c r="F74" s="232" t="s">
+      <c r="E74" s="246"/>
+      <c r="F74" s="318" t="s">
         <v>125</v>
       </c>
-      <c r="G74" s="239"/>
-      <c r="H74" s="269"/>
-      <c r="I74" s="308" t="s">
+      <c r="G74" s="246"/>
+      <c r="H74" s="312"/>
+      <c r="I74" s="286" t="s">
         <v>126</v>
       </c>
-      <c r="J74" s="233"/>
+      <c r="J74" s="237"/>
       <c r="K74" s="6"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
@@ -8543,24 +8543,24 @@
       <c r="AB74" s="3"/>
     </row>
     <row r="75" spans="1:28" ht="69" customHeight="1">
-      <c r="A75" s="256"/>
+      <c r="A75" s="222"/>
       <c r="B75" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C75" s="264"/>
-      <c r="D75" s="279" t="s">
+      <c r="C75" s="282"/>
+      <c r="D75" s="259" t="s">
         <v>88</v>
       </c>
-      <c r="E75" s="239"/>
-      <c r="F75" s="280" t="s">
+      <c r="E75" s="246"/>
+      <c r="F75" s="232" t="s">
         <v>134</v>
       </c>
-      <c r="G75" s="239"/>
-      <c r="H75" s="269"/>
-      <c r="I75" s="236" t="s">
+      <c r="G75" s="246"/>
+      <c r="H75" s="312"/>
+      <c r="I75" s="245" t="s">
         <v>124</v>
       </c>
-      <c r="J75" s="233"/>
+      <c r="J75" s="237"/>
       <c r="K75" s="6"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
@@ -8581,24 +8581,24 @@
       <c r="AB75" s="3"/>
     </row>
     <row r="76" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A76" s="256"/>
+      <c r="A76" s="222"/>
       <c r="B76" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C76" s="264"/>
-      <c r="D76" s="236" t="s">
+      <c r="C76" s="282"/>
+      <c r="D76" s="245" t="s">
         <v>197</v>
       </c>
-      <c r="E76" s="237"/>
-      <c r="F76" s="280" t="s">
+      <c r="E76" s="287"/>
+      <c r="F76" s="232" t="s">
         <v>110</v>
       </c>
-      <c r="G76" s="239"/>
-      <c r="H76" s="269"/>
-      <c r="I76" s="236" t="s">
+      <c r="G76" s="246"/>
+      <c r="H76" s="312"/>
+      <c r="I76" s="245" t="s">
         <v>145</v>
       </c>
-      <c r="J76" s="233"/>
+      <c r="J76" s="237"/>
       <c r="K76" s="6"/>
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
@@ -8619,22 +8619,22 @@
       <c r="AB76" s="3"/>
     </row>
     <row r="77" spans="1:28" ht="57" customHeight="1">
-      <c r="A77" s="256"/>
+      <c r="A77" s="222"/>
       <c r="B77" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C77" s="264"/>
-      <c r="D77" s="227" t="s">
+      <c r="C77" s="282"/>
+      <c r="D77" s="249" t="s">
         <v>243</v>
       </c>
-      <c r="E77" s="237"/>
+      <c r="E77" s="287"/>
       <c r="F77" s="25"/>
       <c r="G77" s="25"/>
-      <c r="H77" s="269"/>
-      <c r="I77" s="227" t="s">
+      <c r="H77" s="312"/>
+      <c r="I77" s="249" t="s">
         <v>242</v>
       </c>
-      <c r="J77" s="233"/>
+      <c r="J77" s="237"/>
       <c r="K77" s="11"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
@@ -8655,24 +8655,24 @@
       <c r="AB77" s="3"/>
     </row>
     <row r="78" spans="1:28" ht="55.5" customHeight="1">
-      <c r="A78" s="256"/>
+      <c r="A78" s="222"/>
       <c r="B78" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C78" s="264"/>
-      <c r="D78" s="279" t="s">
+      <c r="C78" s="282"/>
+      <c r="D78" s="259" t="s">
         <v>89</v>
       </c>
-      <c r="E78" s="239"/>
-      <c r="F78" s="236" t="s">
+      <c r="E78" s="246"/>
+      <c r="F78" s="245" t="s">
         <v>209</v>
       </c>
-      <c r="G78" s="239"/>
-      <c r="H78" s="269"/>
-      <c r="I78" s="236" t="s">
+      <c r="G78" s="246"/>
+      <c r="H78" s="312"/>
+      <c r="I78" s="245" t="s">
         <v>211</v>
       </c>
-      <c r="J78" s="233"/>
+      <c r="J78" s="237"/>
       <c r="K78" s="6"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
@@ -8693,16 +8693,16 @@
       <c r="AB78" s="3"/>
     </row>
     <row r="79" spans="1:28" ht="64.5" hidden="1" customHeight="1">
-      <c r="A79" s="256"/>
+      <c r="A79" s="222"/>
       <c r="B79" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C79" s="264"/>
+      <c r="C79" s="282"/>
       <c r="D79" s="48"/>
       <c r="E79" s="24"/>
       <c r="F79" s="24"/>
       <c r="G79" s="24"/>
-      <c r="H79" s="269"/>
+      <c r="H79" s="312"/>
       <c r="I79" s="36"/>
       <c r="J79" s="77"/>
       <c r="K79" s="6"/>
@@ -8725,24 +8725,24 @@
       <c r="AB79" s="3"/>
     </row>
     <row r="80" spans="1:28" ht="58.5" customHeight="1" thickBot="1">
-      <c r="A80" s="256"/>
+      <c r="A80" s="222"/>
       <c r="B80" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C80" s="265"/>
-      <c r="D80" s="280" t="s">
+      <c r="C80" s="283"/>
+      <c r="D80" s="232" t="s">
         <v>112</v>
       </c>
-      <c r="E80" s="239"/>
-      <c r="F80" s="281" t="s">
+      <c r="E80" s="246"/>
+      <c r="F80" s="308" t="s">
         <v>136</v>
       </c>
-      <c r="G80" s="239"/>
-      <c r="H80" s="269"/>
-      <c r="I80" s="227" t="s">
+      <c r="G80" s="246"/>
+      <c r="H80" s="312"/>
+      <c r="I80" s="249" t="s">
         <v>92</v>
       </c>
-      <c r="J80" s="233"/>
+      <c r="J80" s="237"/>
       <c r="K80" s="6"/>
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
@@ -8763,26 +8763,26 @@
       <c r="AB80" s="3"/>
     </row>
     <row r="81" spans="1:28" ht="50.25" thickBot="1">
-      <c r="A81" s="256"/>
+      <c r="A81" s="222"/>
       <c r="B81" s="18" t="s">
         <v>25</v>
       </c>
       <c r="C81" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="282" t="s">
+      <c r="D81" s="309" t="s">
         <v>117</v>
       </c>
-      <c r="E81" s="283"/>
-      <c r="F81" s="236" t="s">
+      <c r="E81" s="273"/>
+      <c r="F81" s="245" t="s">
         <v>118</v>
       </c>
-      <c r="G81" s="239"/>
-      <c r="H81" s="269"/>
-      <c r="I81" s="276" t="s">
+      <c r="G81" s="246"/>
+      <c r="H81" s="312"/>
+      <c r="I81" s="332" t="s">
         <v>224</v>
       </c>
-      <c r="J81" s="233"/>
+      <c r="J81" s="237"/>
       <c r="K81" s="6"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
@@ -8803,26 +8803,26 @@
       <c r="AB81" s="3"/>
     </row>
     <row r="82" spans="1:28" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A82" s="257"/>
+      <c r="A82" s="223"/>
       <c r="B82" s="78" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D82" s="277" t="s">
+      <c r="D82" s="230" t="s">
         <v>120</v>
       </c>
-      <c r="E82" s="284"/>
-      <c r="F82" s="277" t="s">
+      <c r="E82" s="231"/>
+      <c r="F82" s="230" t="s">
         <v>121</v>
       </c>
-      <c r="G82" s="284"/>
-      <c r="H82" s="270"/>
-      <c r="I82" s="277" t="s">
+      <c r="G82" s="231"/>
+      <c r="H82" s="326"/>
+      <c r="I82" s="230" t="s">
         <v>119</v>
       </c>
-      <c r="J82" s="278"/>
+      <c r="J82" s="333"/>
       <c r="K82" s="6"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
@@ -8844,10 +8844,10 @@
     </row>
     <row r="83" spans="1:28" ht="20.25" thickBot="1">
       <c r="A83" s="191"/>
-      <c r="B83" s="220" t="s">
+      <c r="B83" s="343" t="s">
         <v>50</v>
       </c>
-      <c r="C83" s="221"/>
+      <c r="C83" s="344"/>
       <c r="D83" s="192"/>
       <c r="E83" s="193"/>
       <c r="F83" s="193"/>
@@ -8875,7 +8875,7 @@
       <c r="AB83" s="3"/>
     </row>
     <row r="84" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A84" s="222" t="s">
+      <c r="A84" s="345" t="s">
         <v>50</v>
       </c>
       <c r="B84" s="195" t="s">
@@ -8917,11 +8917,11 @@
       <c r="AB84" s="3"/>
     </row>
     <row r="85" spans="1:28" ht="66">
-      <c r="A85" s="223"/>
+      <c r="A85" s="346"/>
       <c r="B85" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="225"/>
+      <c r="C85" s="348"/>
       <c r="D85" s="108" t="s">
         <v>204</v>
       </c>
@@ -8953,11 +8953,11 @@
       <c r="AB85" s="3"/>
     </row>
     <row r="86" spans="1:28" ht="66">
-      <c r="A86" s="223"/>
+      <c r="A86" s="346"/>
       <c r="B86" s="202" t="s">
         <v>17</v>
       </c>
-      <c r="C86" s="226"/>
+      <c r="C86" s="349"/>
       <c r="D86" s="109" t="s">
         <v>127</v>
       </c>
@@ -8989,11 +8989,11 @@
       <c r="AB86" s="3"/>
     </row>
     <row r="87" spans="1:28" ht="49.5">
-      <c r="A87" s="223"/>
+      <c r="A87" s="346"/>
       <c r="B87" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="C87" s="226"/>
+      <c r="C87" s="349"/>
       <c r="D87" s="188" t="s">
         <v>257</v>
       </c>
@@ -9025,11 +9025,11 @@
       <c r="AB87" s="3"/>
     </row>
     <row r="88" spans="1:28" ht="66">
-      <c r="A88" s="223"/>
+      <c r="A88" s="346"/>
       <c r="B88" s="202" t="s">
         <v>19</v>
       </c>
-      <c r="C88" s="226"/>
+      <c r="C88" s="349"/>
       <c r="D88" s="188" t="s">
         <v>256</v>
       </c>
@@ -9061,11 +9061,11 @@
       <c r="AB88" s="3"/>
     </row>
     <row r="89" spans="1:28" ht="49.5">
-      <c r="A89" s="223"/>
+      <c r="A89" s="346"/>
       <c r="B89" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="C89" s="226"/>
+      <c r="C89" s="349"/>
       <c r="D89" s="109" t="s">
         <v>268</v>
       </c>
@@ -9077,8 +9077,8 @@
       </c>
       <c r="G89" s="179"/>
       <c r="H89" s="189"/>
-      <c r="I89" s="227"/>
-      <c r="J89" s="228"/>
+      <c r="I89" s="220"/>
+      <c r="J89" s="213"/>
       <c r="K89" s="1"/>
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
@@ -9099,7 +9099,7 @@
       <c r="AB89" s="3"/>
     </row>
     <row r="90" spans="1:28" ht="50.25" thickBot="1">
-      <c r="A90" s="223"/>
+      <c r="A90" s="346"/>
       <c r="B90" s="210" t="s">
         <v>23</v>
       </c>
@@ -9114,8 +9114,8 @@
       <c r="G90" s="184" t="s">
         <v>267</v>
       </c>
-      <c r="H90" s="227"/>
-      <c r="I90" s="229"/>
+      <c r="H90" s="220"/>
+      <c r="I90" s="220"/>
       <c r="J90" s="213"/>
       <c r="K90" s="1"/>
       <c r="L90" s="2"/>
@@ -9137,7 +9137,7 @@
       <c r="AB90" s="3"/>
     </row>
     <row r="91" spans="1:28" ht="32.25" thickBot="1">
-      <c r="A91" s="224"/>
+      <c r="A91" s="347"/>
       <c r="B91" s="210" t="s">
         <v>24</v>
       </c>
@@ -9146,8 +9146,8 @@
       <c r="E91" s="216"/>
       <c r="F91" s="216"/>
       <c r="G91" s="215"/>
-      <c r="H91" s="230"/>
-      <c r="I91" s="231"/>
+      <c r="H91" s="351"/>
+      <c r="I91" s="352"/>
       <c r="J91" s="217"/>
       <c r="K91" s="1"/>
       <c r="L91" s="2"/>
@@ -9170,10 +9170,10 @@
     </row>
     <row r="92" spans="1:28" ht="20.25" thickBot="1">
       <c r="A92" s="191"/>
-      <c r="B92" s="220" t="s">
+      <c r="B92" s="343" t="s">
         <v>60</v>
       </c>
-      <c r="C92" s="221"/>
+      <c r="C92" s="344"/>
       <c r="D92" s="192"/>
       <c r="E92" s="193"/>
       <c r="F92" s="193"/>
@@ -9201,7 +9201,7 @@
       <c r="AB92" s="3"/>
     </row>
     <row r="93" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A93" s="222" t="s">
+      <c r="A93" s="345" t="s">
         <v>60</v>
       </c>
       <c r="B93" s="195" t="s">
@@ -9241,11 +9241,11 @@
       <c r="AB93" s="3"/>
     </row>
     <row r="94" spans="1:28" ht="66">
-      <c r="A94" s="223"/>
+      <c r="A94" s="346"/>
       <c r="B94" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="C94" s="225"/>
+      <c r="C94" s="348"/>
       <c r="D94" s="118" t="s">
         <v>207</v>
       </c>
@@ -9277,11 +9277,11 @@
       <c r="AB94" s="3"/>
     </row>
     <row r="95" spans="1:28" ht="66">
-      <c r="A95" s="223"/>
+      <c r="A95" s="346"/>
       <c r="B95" s="202" t="s">
         <v>17</v>
       </c>
-      <c r="C95" s="226"/>
+      <c r="C95" s="349"/>
       <c r="D95" s="109" t="s">
         <v>129</v>
       </c>
@@ -9313,11 +9313,11 @@
       <c r="AB95" s="3"/>
     </row>
     <row r="96" spans="1:28" ht="49.5">
-      <c r="A96" s="223"/>
+      <c r="A96" s="346"/>
       <c r="B96" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="C96" s="226"/>
+      <c r="C96" s="349"/>
       <c r="D96" s="188" t="s">
         <v>259</v>
       </c>
@@ -9351,11 +9351,11 @@
       <c r="AB96" s="3"/>
     </row>
     <row r="97" spans="1:28" ht="49.5">
-      <c r="A97" s="223"/>
+      <c r="A97" s="346"/>
       <c r="B97" s="202" t="s">
         <v>19</v>
       </c>
-      <c r="C97" s="226"/>
+      <c r="C97" s="349"/>
       <c r="D97" s="109" t="s">
         <v>131</v>
       </c>
@@ -9387,11 +9387,11 @@
       <c r="AB97" s="3"/>
     </row>
     <row r="98" spans="1:28" ht="66.75" thickBot="1">
-      <c r="A98" s="223"/>
+      <c r="A98" s="346"/>
       <c r="B98" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="C98" s="226"/>
+      <c r="C98" s="349"/>
       <c r="D98" s="212" t="s">
         <v>265</v>
       </c>
@@ -9401,8 +9401,8 @@
       <c r="F98" s="219"/>
       <c r="G98" s="209"/>
       <c r="H98" s="189"/>
-      <c r="I98" s="227"/>
-      <c r="J98" s="228"/>
+      <c r="I98" s="249"/>
+      <c r="J98" s="350"/>
       <c r="K98" s="1"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
@@ -9424,8 +9424,8 @@
     </row>
     <row r="99" spans="1:28" ht="19.5">
       <c r="A99" s="191"/>
-      <c r="B99" s="220"/>
-      <c r="C99" s="221"/>
+      <c r="B99" s="343"/>
+      <c r="C99" s="344"/>
       <c r="D99" s="192"/>
       <c r="E99" s="193"/>
       <c r="F99" s="193"/>
@@ -36453,7 +36453,138 @@
       <c r="AB999" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="157">
+  <mergeCells count="155">
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="A84:A91"/>
+    <mergeCell ref="C85:C89"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="A93:A98"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A68:A82"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="C72:C80"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H69:H82"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="I80:J80"/>
+    <mergeCell ref="I81:J81"/>
+    <mergeCell ref="I82:J82"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="C41:C49"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="A37:A51"/>
+    <mergeCell ref="A53:A66"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="G1:J2"/>
+    <mergeCell ref="A2:E4"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C10:C20"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="A22:A35"/>
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="D35:E35"/>
@@ -36478,139 +36609,6 @@
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="G1:J2"/>
-    <mergeCell ref="A2:E4"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C10:C20"/>
-    <mergeCell ref="A7:A20"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="A37:A51"/>
-    <mergeCell ref="A53:A66"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C41:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="A68:A82"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="C72:C80"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H69:H82"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="I78:J78"/>
-    <mergeCell ref="I80:J80"/>
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="I82:J82"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="A84:A91"/>
-    <mergeCell ref="C85:C89"/>
-    <mergeCell ref="I89:J89"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="A93:A98"/>
-    <mergeCell ref="C94:C98"/>
-    <mergeCell ref="I98:J98"/>
   </mergeCells>
   <pageMargins left="0.216187305364964" right="0.14099172089019399" top="0.26" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="25" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>